<commit_message>
week 3 schedule inputs
</commit_message>
<xml_diff>
--- a/data/Fall2022Schedule.xlsx
+++ b/data/Fall2022Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BC9EC4-B1E9-4EF3-A5BE-C2EF048ACE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52193ECC-8576-413C-8C01-9B7F7E086074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32160" yWindow="4065" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
+    <workbookView xWindow="2595" yWindow="1350" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Wookie Mistakes" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="36">
   <si>
     <t>Record</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>470-646-4492</t>
+  </si>
+  <si>
+    <t>Shelia Lowe</t>
+  </si>
+  <si>
+    <t>205-960-0472</t>
   </si>
 </sst>
 </file>
@@ -229,42 +235,13 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -574,11 +551,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA30A97-9145-4EDA-8DB9-44B6A1233BAB}">
-  <dimension ref="A2:W22"/>
+  <dimension ref="A2:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,70 +579,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="1">
         <v>44804</v>
       </c>
       <c r="C2" s="1">
-        <f>B2+7</f>
+        <f t="shared" ref="C2:Q2" si="0">B2+7</f>
         <v>44811</v>
       </c>
       <c r="D2" s="1">
-        <f>C2+7</f>
+        <f t="shared" si="0"/>
         <v>44818</v>
       </c>
       <c r="E2" s="1">
-        <f>D2+7</f>
+        <f t="shared" si="0"/>
         <v>44825</v>
       </c>
       <c r="F2" s="1">
-        <f>E2+7</f>
+        <f t="shared" si="0"/>
         <v>44832</v>
       </c>
       <c r="G2" s="1">
-        <f>F2+7</f>
+        <f t="shared" si="0"/>
         <v>44839</v>
       </c>
       <c r="H2" s="1">
-        <f>G2+7</f>
+        <f t="shared" si="0"/>
         <v>44846</v>
       </c>
       <c r="I2" s="1">
-        <f>H2+7</f>
+        <f t="shared" si="0"/>
         <v>44853</v>
       </c>
       <c r="J2" s="1">
-        <f>I2+7</f>
+        <f t="shared" si="0"/>
         <v>44860</v>
       </c>
       <c r="K2" s="1">
-        <f>J2+7</f>
+        <f t="shared" si="0"/>
         <v>44867</v>
       </c>
       <c r="L2" s="1">
-        <f>K2+7</f>
+        <f t="shared" si="0"/>
         <v>44874</v>
       </c>
       <c r="M2" s="1">
-        <f>L2+7</f>
+        <f t="shared" si="0"/>
         <v>44881</v>
       </c>
       <c r="N2" s="1">
-        <f>M2+7</f>
+        <f t="shared" si="0"/>
         <v>44888</v>
       </c>
       <c r="O2" s="1">
-        <f>N2+7</f>
+        <f t="shared" si="0"/>
         <v>44895</v>
       </c>
       <c r="P2" s="1">
-        <f>O2+7</f>
+        <f t="shared" si="0"/>
         <v>44902</v>
       </c>
       <c r="Q2" s="1">
-        <f>P2+7</f>
+        <f t="shared" si="0"/>
         <v>44909</v>
       </c>
       <c r="R2" s="3" t="s">
@@ -695,10 +672,10 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
@@ -740,23 +717,23 @@
         <v>25</v>
       </c>
       <c r="R3" s="6">
-        <f>COUNTIF(B3:O3, "W")/(COUNTIF(B3:O3, "W")+COUNTIF(B3:O3, "L"))</f>
-        <v>1</v>
+        <f t="shared" ref="R3:R10" si="1">COUNTIF(B3:O3, "W")/(COUNTIF(B3:O3, "W")+COUNTIF(B3:O3, "L"))</f>
+        <v>0.5</v>
       </c>
       <c r="S3">
         <v>10</v>
       </c>
       <c r="T3">
-        <f>S3-COUNTIF(B3:Q3, "W")-COUNTIF(B3:Q3, "L")</f>
-        <v>9</v>
+        <f t="shared" ref="T3:T10" si="2">S3-COUNTIF(B3:Q3, "W")-COUNTIF(B3:Q3, "L")</f>
+        <v>8</v>
       </c>
       <c r="U3">
-        <f>COUNTIF(B3:Q3, "A")</f>
-        <v>15</v>
+        <f t="shared" ref="U3:U10" si="3">COUNTIF(B3:Q3, "A")</f>
+        <v>13</v>
       </c>
       <c r="V3">
-        <f>U3-T3</f>
-        <v>6</v>
+        <f t="shared" ref="V3:V10" si="4">U3-T3</f>
+        <v>5</v>
       </c>
       <c r="W3" t="s">
         <v>28</v>
@@ -770,10 +747,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -814,23 +791,23 @@
       <c r="Q4" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="6" t="e">
-        <f>COUNTIF(B4:O4, "W")/(COUNTIF(B4:O4, "W")+COUNTIF(B4:O4, "L"))</f>
-        <v>#DIV/0!</v>
+      <c r="R4" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="S4">
         <v>6</v>
       </c>
       <c r="T4">
-        <f>S4-COUNTIF(B4:Q4, "W")-COUNTIF(B4:Q4, "L")</f>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="U4">
-        <f>COUNTIF(B4:Q4, "A")</f>
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
       <c r="V4">
-        <f>U4-T4</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="W4" t="s">
@@ -845,10 +822,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -889,24 +866,24 @@
       <c r="Q5" t="s">
         <v>25</v>
       </c>
-      <c r="R5" s="6" t="e">
-        <f>COUNTIF(B5:O5, "W")/(COUNTIF(B5:O5, "W")+COUNTIF(B5:O5, "L"))</f>
-        <v>#DIV/0!</v>
+      <c r="R5" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="S5">
         <v>6</v>
       </c>
       <c r="T5">
-        <f>S5-COUNTIF(B5:Q5, "W")-COUNTIF(B5:Q5, "L")</f>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="U5">
-        <f>COUNTIF(B5:Q5, "A")</f>
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
       <c r="V5">
-        <f>U5-T5</f>
-        <v>9</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="W5" t="s">
         <v>9</v>
@@ -920,10 +897,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>
@@ -964,23 +941,23 @@
       <c r="Q6" t="s">
         <v>25</v>
       </c>
-      <c r="R6" s="6" t="e">
-        <f>COUNTIF(B6:O6, "W")/(COUNTIF(B6:O6, "W")+COUNTIF(B6:O6, "L"))</f>
-        <v>#DIV/0!</v>
+      <c r="R6" s="6">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="S6">
         <v>6</v>
       </c>
       <c r="T6">
-        <f>S6-COUNTIF(B6:Q6, "W")-COUNTIF(B6:Q6, "L")</f>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="U6">
-        <f>COUNTIF(B6:Q6, "A")</f>
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
       <c r="V6">
-        <f>U6-T6</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="W6" t="s">
@@ -995,10 +972,10 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
@@ -1040,23 +1017,23 @@
         <v>25</v>
       </c>
       <c r="R7" s="6">
-        <f>COUNTIF(B7:O7, "W")/(COUNTIF(B7:O7, "W")+COUNTIF(B7:O7, "L"))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="S7" s="8">
+      <c r="S7">
         <v>6</v>
       </c>
       <c r="T7">
-        <f>S7-COUNTIF(B7:Q7, "W")-COUNTIF(B7:Q7, "L")</f>
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="U7">
-        <f>COUNTIF(B7:Q7, "A")</f>
-        <v>15</v>
-      </c>
-      <c r="V7" s="8">
-        <f>U7-T7</f>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="4"/>
+        <v>9</v>
       </c>
       <c r="W7" t="s">
         <v>20</v>
@@ -1070,10 +1047,10 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
         <v>25</v>
@@ -1115,23 +1092,23 @@
         <v>25</v>
       </c>
       <c r="R8" s="6">
-        <f>COUNTIF(B8:O8, "W")/(COUNTIF(B8:O8, "W")+COUNTIF(B8:O8, "L"))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="S8">
         <v>6</v>
       </c>
       <c r="T8">
-        <f>S8-COUNTIF(B8:Q8, "W")-COUNTIF(B8:Q8, "L")</f>
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="U8">
-        <f>COUNTIF(B8:Q8, "A")</f>
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
       <c r="V8">
-        <f>U8-T8</f>
-        <v>10</v>
+        <f t="shared" si="4"/>
+        <v>9</v>
       </c>
       <c r="W8" t="s">
         <v>15</v>
@@ -1145,10 +1122,10 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
@@ -1190,23 +1167,23 @@
         <v>25</v>
       </c>
       <c r="R9" s="6">
-        <f>COUNTIF(B9:O9, "W")/(COUNTIF(B9:O9, "W")+COUNTIF(B9:O9, "L"))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="S9">
         <v>6</v>
       </c>
       <c r="T9">
-        <f>S9-COUNTIF(B9:Q9, "W")-COUNTIF(B9:Q9, "L")</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="U9">
-        <f>COUNTIF(B9:Q9, "A")</f>
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
       <c r="V9">
-        <f>U9-T9</f>
-        <v>10</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="W9" t="s">
         <v>13</v>
@@ -1220,10 +1197,10 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
@@ -1265,22 +1242,22 @@
         <v>25</v>
       </c>
       <c r="R10" s="6">
-        <f>COUNTIF(B10:O10, "W")/(COUNTIF(B10:O10, "W")+COUNTIF(B10:O10, "L"))</f>
-        <v>1</v>
-      </c>
-      <c r="S10" s="8">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="S10">
         <v>6</v>
       </c>
-      <c r="T10" s="8">
-        <f>S10-COUNTIF(B10:Q10, "W")-COUNTIF(B10:Q10, "L")</f>
-        <v>5</v>
-      </c>
-      <c r="U10" s="8">
-        <f>COUNTIF(B10:Q10, "A")</f>
-        <v>15</v>
-      </c>
-      <c r="V10" s="8">
-        <f>U10-T10</f>
+      <c r="T10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="W10" t="s">
@@ -1292,72 +1269,72 @@
         <v>23</v>
       </c>
       <c r="B11" s="5">
-        <f>COUNTIF(B3:B10, "W")/(COUNTIF(B3:B10, "W")+COUNTIF(B3:B10, "L"))</f>
+        <f t="shared" ref="B11:Q11" si="5">COUNTIF(B3:B10, "W")/(COUNTIF(B3:B10, "W")+COUNTIF(B3:B10, "L"))</f>
         <v>1</v>
       </c>
-      <c r="C11" s="5" t="e">
-        <f>COUNTIF(C3:C10, "W")/(COUNTIF(C3:C10, "W")+COUNTIF(C3:C10, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D11" s="5" t="e">
-        <f>COUNTIF(D3:D10, "W")/(COUNTIF(D3:D10, "W")+COUNTIF(D3:D10, "L"))</f>
-        <v>#DIV/0!</v>
+      <c r="C11" s="5">
+        <f t="shared" si="5"/>
+        <v>0.2</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="5"/>
+        <v>0.6</v>
       </c>
       <c r="E11" s="5" t="e">
-        <f>COUNTIF(E3:E10, "W")/(COUNTIF(E3:E10, "W")+COUNTIF(E3:E10, "L"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F11" s="5" t="e">
-        <f>COUNTIF(F3:F10, "W")/(COUNTIF(F3:F10, "W")+COUNTIF(F3:F10, "L"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G11" s="5" t="e">
-        <f>COUNTIF(G3:G10, "W")/(COUNTIF(G3:G10, "W")+COUNTIF(G3:G10, "L"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H11" s="5" t="e">
-        <f>COUNTIF(H3:H10, "W")/(COUNTIF(H3:H10, "W")+COUNTIF(H3:H10, "L"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I11" s="5" t="e">
-        <f>COUNTIF(I3:I10, "W")/(COUNTIF(I3:I10, "W")+COUNTIF(I3:I10, "L"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J11" s="5" t="e">
-        <f>COUNTIF(J3:J10, "W")/(COUNTIF(J3:J10, "W")+COUNTIF(J3:J10, "L"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K11" s="5" t="e">
-        <f>COUNTIF(K3:K10, "W")/(COUNTIF(K3:K10, "W")+COUNTIF(K3:K10, "L"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L11" s="5" t="e">
-        <f>COUNTIF(L3:L10, "W")/(COUNTIF(L3:L10, "W")+COUNTIF(L3:L10, "L"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M11" s="5" t="e">
-        <f>COUNTIF(M3:M10, "W")/(COUNTIF(M3:M10, "W")+COUNTIF(M3:M10, "L"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N11" s="5" t="e">
-        <f>COUNTIF(N3:N10, "W")/(COUNTIF(N3:N10, "W")+COUNTIF(N3:N10, "L"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O11" s="5" t="e">
-        <f>COUNTIF(O3:O10, "W")/(COUNTIF(O3:O10, "W")+COUNTIF(O3:O10, "L"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P11" s="5" t="e">
-        <f>COUNTIF(P3:P10, "W")/(COUNTIF(P3:P10, "W")+COUNTIF(P3:P10, "L"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q11" s="5" t="e">
-        <f>COUNTIF(Q3:Q10, "W")/(COUNTIF(Q3:Q10, "W")+COUNTIF(Q3:Q10, "L"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R11" s="7">
         <f>AVERAGEIF(B11:O11, "&gt;=0")</f>
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="S11" s="2">
         <f>SUM(S3:S10)</f>
@@ -1365,82 +1342,82 @@
       </c>
       <c r="T11" s="2">
         <f>SUM(T3:T10)</f>
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="U11" s="2">
         <f>SUM(U3:U10)</f>
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="V11" s="2">
         <f>SUM(V3:V10)</f>
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="1">
         <v>44804</v>
       </c>
       <c r="C14" s="1">
-        <f>B14+7</f>
+        <f t="shared" ref="C14:Q14" si="6">B14+7</f>
         <v>44811</v>
       </c>
       <c r="D14" s="1">
-        <f>C14+7</f>
+        <f t="shared" si="6"/>
         <v>44818</v>
       </c>
       <c r="E14" s="1">
-        <f>D14+7</f>
+        <f t="shared" si="6"/>
         <v>44825</v>
       </c>
       <c r="F14" s="1">
-        <f>E14+7</f>
+        <f t="shared" si="6"/>
         <v>44832</v>
       </c>
       <c r="G14" s="1">
-        <f>F14+7</f>
+        <f t="shared" si="6"/>
         <v>44839</v>
       </c>
       <c r="H14" s="1">
-        <f>G14+7</f>
+        <f t="shared" si="6"/>
         <v>44846</v>
       </c>
       <c r="I14" s="1">
-        <f>H14+7</f>
+        <f t="shared" si="6"/>
         <v>44853</v>
       </c>
       <c r="J14" s="1">
-        <f>I14+7</f>
+        <f t="shared" si="6"/>
         <v>44860</v>
       </c>
       <c r="K14" s="1">
-        <f>J14+7</f>
+        <f t="shared" si="6"/>
         <v>44867</v>
       </c>
       <c r="L14" s="1">
-        <f>K14+7</f>
+        <f t="shared" si="6"/>
         <v>44874</v>
       </c>
       <c r="M14" s="1">
-        <f>L14+7</f>
+        <f t="shared" si="6"/>
         <v>44881</v>
       </c>
       <c r="N14" s="1">
-        <f>M14+7</f>
+        <f t="shared" si="6"/>
         <v>44888</v>
       </c>
       <c r="O14" s="1">
-        <f>N14+7</f>
+        <f t="shared" si="6"/>
         <v>44895</v>
       </c>
       <c r="P14" s="1">
-        <f>O14+7</f>
+        <f t="shared" si="6"/>
         <v>44902</v>
       </c>
       <c r="Q14" s="1">
-        <f>P14+7</f>
+        <f t="shared" si="6"/>
         <v>44909</v>
       </c>
       <c r="R14" s="3" t="s">
@@ -1470,10 +1447,10 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
@@ -1514,24 +1491,24 @@
       <c r="Q15" t="s">
         <v>25</v>
       </c>
-      <c r="R15" s="6" t="e">
-        <f>COUNTIF(B15:O15, "W")/(COUNTIF(B15:O15, "W")+COUNTIF(B15:O15, "L"))</f>
-        <v>#DIV/0!</v>
+      <c r="R15" s="6">
+        <f t="shared" ref="R15:R20" si="7">COUNTIF(B15:O15, "W")/(COUNTIF(B15:O15, "W")+COUNTIF(B15:O15, "L"))</f>
+        <v>1</v>
       </c>
       <c r="S15">
         <v>10</v>
       </c>
       <c r="T15">
-        <f>S15-COUNTIF(B15:Q15, "W")-COUNTIF(B15:Q15, "L")</f>
-        <v>10</v>
+        <f t="shared" ref="T15:T20" si="8">S15-COUNTIF(B15:Q15, "W")-COUNTIF(B15:Q15, "L")</f>
+        <v>9</v>
       </c>
       <c r="U15">
-        <f>COUNTIF(B15:Q15, "A")</f>
-        <v>15</v>
+        <f t="shared" ref="U15:U20" si="9">COUNTIF(B15:Q15, "A")</f>
+        <v>13</v>
       </c>
       <c r="V15">
-        <f>U15-T15</f>
-        <v>5</v>
+        <f t="shared" ref="V15:V20" si="10">U15-T15</f>
+        <v>4</v>
       </c>
       <c r="W15" t="s">
         <v>13</v>
@@ -1545,10 +1522,10 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
@@ -1590,22 +1567,22 @@
         <v>25</v>
       </c>
       <c r="R16" s="6">
-        <f>COUNTIF(B16:O16, "W")/(COUNTIF(B16:O16, "W")+COUNTIF(B16:O16, "L"))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S16">
         <v>10</v>
       </c>
       <c r="T16">
-        <f>S16-COUNTIF(B16:Q16, "W")-COUNTIF(B16:Q16, "L")</f>
-        <v>9</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
       </c>
       <c r="U16">
-        <f>COUNTIF(B16:Q16, "A")</f>
-        <v>15</v>
+        <f t="shared" si="9"/>
+        <v>13</v>
       </c>
       <c r="V16">
-        <f>U16-T16</f>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="W16" t="s">
@@ -1620,10 +1597,10 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s">
         <v>25</v>
@@ -1665,23 +1642,23 @@
         <v>25</v>
       </c>
       <c r="R17" s="6">
-        <f>COUNTIF(B17:O17, "W")/(COUNTIF(B17:O17, "W")+COUNTIF(B17:O17, "L"))</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>0.5</v>
       </c>
       <c r="S17">
         <v>10</v>
       </c>
       <c r="T17">
-        <f>S17-COUNTIF(B17:Q17, "W")-COUNTIF(B17:Q17, "L")</f>
-        <v>9</v>
+        <f t="shared" si="8"/>
+        <v>8</v>
       </c>
       <c r="U17">
-        <f>COUNTIF(B17:Q17, "A")</f>
-        <v>15</v>
+        <f t="shared" si="9"/>
+        <v>13</v>
       </c>
       <c r="V17">
-        <f>U17-T17</f>
-        <v>6</v>
+        <f t="shared" si="10"/>
+        <v>5</v>
       </c>
       <c r="W17" t="s">
         <v>28</v>
@@ -1695,10 +1672,10 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
@@ -1740,22 +1717,22 @@
         <v>25</v>
       </c>
       <c r="R18" s="6">
-        <f>COUNTIF(B18:O18, "W")/(COUNTIF(B18:O18, "W")+COUNTIF(B18:O18, "L"))</f>
-        <v>0</v>
-      </c>
-      <c r="S18" s="8">
+        <f t="shared" si="7"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="S18">
         <v>10</v>
       </c>
       <c r="T18">
-        <f>S18-COUNTIF(B18:Q18, "W")-COUNTIF(B18:Q18, "L")</f>
-        <v>9</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
       </c>
       <c r="U18">
-        <f>COUNTIF(B18:Q18, "A")</f>
-        <v>15</v>
-      </c>
-      <c r="V18" s="8">
-        <f>U18-T18</f>
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="W18" t="s">
@@ -1766,72 +1743,72 @@
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q19" s="8" t="s">
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" t="s">
+        <v>25</v>
+      </c>
+      <c r="N19" t="s">
+        <v>25</v>
+      </c>
+      <c r="O19" t="s">
+        <v>25</v>
+      </c>
+      <c r="P19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q19" t="s">
         <v>25</v>
       </c>
       <c r="R19" s="6">
-        <f>COUNTIF(B19:O19, "W")/(COUNTIF(B19:O19, "W")+COUNTIF(B19:O19, "L"))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S19" s="8">
+      <c r="S19">
         <v>10</v>
       </c>
-      <c r="T19" s="8">
-        <f>S19-COUNTIF(B19:Q19, "W")-COUNTIF(B19:Q19, "L")</f>
-        <v>9</v>
-      </c>
-      <c r="U19" s="8">
-        <f>COUNTIF(B19:Q19, "A")</f>
-        <v>15</v>
-      </c>
-      <c r="V19" s="8">
-        <f>U19-T19</f>
-        <v>6</v>
+      <c r="T19">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="10"/>
+        <v>5</v>
       </c>
       <c r="W19" t="s">
         <v>22</v>
@@ -1845,10 +1822,10 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
@@ -1889,24 +1866,24 @@
       <c r="Q20" t="s">
         <v>25</v>
       </c>
-      <c r="R20" s="6" t="e">
-        <f>COUNTIF(B20:O20, "W")/(COUNTIF(B20:O20, "W")+COUNTIF(B20:O20, "L"))</f>
-        <v>#DIV/0!</v>
+      <c r="R20" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="S20">
         <v>6</v>
       </c>
       <c r="T20">
-        <f>S20-COUNTIF(B20:Q20, "W")-COUNTIF(B20:Q20, "L")</f>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="U20">
-        <f>COUNTIF(B20:Q20, "A")</f>
-        <v>15</v>
+        <f t="shared" si="9"/>
+        <v>13</v>
       </c>
       <c r="V20">
-        <f>U20-T20</f>
-        <v>9</v>
+        <f t="shared" si="10"/>
+        <v>8</v>
       </c>
       <c r="W20" t="s">
         <v>33</v>
@@ -1920,10 +1897,10 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
@@ -1973,107 +1950,182 @@
       </c>
       <c r="T21">
         <f>S21-COUNTIF(B21:Q21, "W")-COUNTIF(B21:Q21, "L")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U21">
         <f>COUNTIF(B21:Q21, "A")</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V21">
         <f>U21-T21</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W21" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22" t="s">
+        <v>25</v>
+      </c>
+      <c r="N22" t="s">
+        <v>25</v>
+      </c>
+      <c r="O22" t="s">
+        <v>25</v>
+      </c>
+      <c r="P22" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>25</v>
+      </c>
+      <c r="R22" s="6">
+        <f>COUNTIF(B22:O22, "W")/(COUNTIF(B22:O22, "W")+COUNTIF(B22:O22, "L"))</f>
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>10</v>
+      </c>
+      <c r="T22">
+        <f>S22-COUNTIF(B22:Q22, "W")-COUNTIF(B22:Q22, "L")</f>
+        <v>9</v>
+      </c>
+      <c r="U22">
+        <f>COUNTIF(B22:Q22, "A")</f>
+        <v>13</v>
+      </c>
+      <c r="V22">
+        <f>U22-T22</f>
+        <v>4</v>
+      </c>
+      <c r="W22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="5">
-        <f>COUNTIF(B15:B21, "W")/(COUNTIF(B15:B21, "W")+COUNTIF(B15:B21, "L"))</f>
+      <c r="B23" s="5">
+        <f>COUNTIF(B15:B22, "W")/(COUNTIF(B15:B22, "W")+COUNTIF(B15:B22, "L"))</f>
         <v>0.4</v>
       </c>
-      <c r="C22" s="5" t="e">
-        <f>COUNTIF(C15:C21, "W")/(COUNTIF(C15:C21, "W")+COUNTIF(C15:C21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D22" s="5" t="e">
-        <f>COUNTIF(D15:D21, "W")/(COUNTIF(D15:D21, "W")+COUNTIF(D15:D21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E22" s="5" t="e">
-        <f>COUNTIF(E15:E21, "W")/(COUNTIF(E15:E21, "W")+COUNTIF(E15:E21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F22" s="5" t="e">
-        <f>COUNTIF(F15:F21, "W")/(COUNTIF(F15:F21, "W")+COUNTIF(F15:F21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G22" s="5" t="e">
-        <f>COUNTIF(G15:G21, "W")/(COUNTIF(G15:G21, "W")+COUNTIF(G15:G21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H22" s="5" t="e">
-        <f>COUNTIF(H15:H21, "W")/(COUNTIF(H15:H21, "W")+COUNTIF(H15:H21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I22" s="5" t="e">
-        <f>COUNTIF(I15:I21, "W")/(COUNTIF(I15:I21, "W")+COUNTIF(I15:I21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J22" s="5" t="e">
-        <f>COUNTIF(J15:J21, "W")/(COUNTIF(J15:J21, "W")+COUNTIF(J15:J21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K22" s="5" t="e">
-        <f>COUNTIF(K15:K21, "W")/(COUNTIF(K15:K21, "W")+COUNTIF(K15:K21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L22" s="5" t="e">
-        <f>COUNTIF(L15:L21, "W")/(COUNTIF(L15:L21, "W")+COUNTIF(L15:L21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M22" s="5" t="e">
-        <f>COUNTIF(M15:M21, "W")/(COUNTIF(M15:M21, "W")+COUNTIF(M15:M21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N22" s="5" t="e">
-        <f>COUNTIF(N15:N21, "W")/(COUNTIF(N15:N21, "W")+COUNTIF(N15:N21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O22" s="5" t="e">
-        <f>COUNTIF(O15:O21, "W")/(COUNTIF(O15:O21, "W")+COUNTIF(O15:O21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P22" s="5" t="e">
-        <f>COUNTIF(P15:P21, "W")/(COUNTIF(P15:P21, "W")+COUNTIF(P15:P21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q22" s="5" t="e">
-        <f>COUNTIF(Q15:Q21, "W")/(COUNTIF(Q15:Q21, "W")+COUNTIF(Q15:Q21, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R22" s="7">
-        <f>AVERAGEIF(B22:O22, "&gt;=0")</f>
-        <v>0.4</v>
-      </c>
-      <c r="S22" s="2">
-        <f>SUM(S15:S21)</f>
-        <v>62</v>
-      </c>
-      <c r="T22" s="2">
-        <f>SUM(T15:T21)</f>
+      <c r="C23" s="5">
+        <f t="shared" ref="C23:D23" si="11">COUNTIF(C15:C22, "W")/(COUNTIF(C15:C22, "W")+COUNTIF(C15:C22, "L"))</f>
+        <v>0.6</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="11"/>
+        <v>0.6</v>
+      </c>
+      <c r="E23" s="5" t="e">
+        <f t="shared" ref="E23" si="12">COUNTIF(E15:E22, "W")/(COUNTIF(E15:E22, "W")+COUNTIF(E15:E22, "L"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F23" s="5" t="e">
+        <f t="shared" ref="F23" si="13">COUNTIF(F15:F22, "W")/(COUNTIF(F15:F22, "W")+COUNTIF(F15:F22, "L"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G23" s="5" t="e">
+        <f t="shared" ref="G23" si="14">COUNTIF(G15:G22, "W")/(COUNTIF(G15:G22, "W")+COUNTIF(G15:G22, "L"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" s="5" t="e">
+        <f t="shared" ref="H23" si="15">COUNTIF(H15:H22, "W")/(COUNTIF(H15:H22, "W")+COUNTIF(H15:H22, "L"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" s="5" t="e">
+        <f t="shared" ref="I23" si="16">COUNTIF(I15:I22, "W")/(COUNTIF(I15:I22, "W")+COUNTIF(I15:I22, "L"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J23" s="5" t="e">
+        <f t="shared" ref="J23" si="17">COUNTIF(J15:J22, "W")/(COUNTIF(J15:J22, "W")+COUNTIF(J15:J22, "L"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K23" s="5" t="e">
+        <f t="shared" ref="K23" si="18">COUNTIF(K15:K22, "W")/(COUNTIF(K15:K22, "W")+COUNTIF(K15:K22, "L"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L23" s="5" t="e">
+        <f t="shared" ref="L23" si="19">COUNTIF(L15:L22, "W")/(COUNTIF(L15:L22, "W")+COUNTIF(L15:L22, "L"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M23" s="5" t="e">
+        <f t="shared" ref="M23" si="20">COUNTIF(M15:M22, "W")/(COUNTIF(M15:M22, "W")+COUNTIF(M15:M22, "L"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N23" s="5" t="e">
+        <f t="shared" ref="N23" si="21">COUNTIF(N15:N22, "W")/(COUNTIF(N15:N22, "W")+COUNTIF(N15:N22, "L"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O23" s="5" t="e">
+        <f t="shared" ref="O23" si="22">COUNTIF(O15:O22, "W")/(COUNTIF(O15:O22, "W")+COUNTIF(O15:O22, "L"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P23" s="5" t="e">
+        <f t="shared" ref="P23" si="23">COUNTIF(P15:P22, "W")/(COUNTIF(P15:P22, "W")+COUNTIF(P15:P22, "L"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q23" s="5" t="e">
+        <f t="shared" ref="Q23" si="24">COUNTIF(Q15:Q22, "W")/(COUNTIF(Q15:Q22, "W")+COUNTIF(Q15:Q22, "L"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R23" s="7">
+        <f>AVERAGEIF(B23:O23, "&gt;=0")</f>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="S23" s="2">
+        <f>SUM(S15:S22)</f>
+        <v>72</v>
+      </c>
+      <c r="T23" s="2">
+        <f>SUM(T15:T22)</f>
         <v>57</v>
       </c>
-      <c r="U22" s="2">
-        <f>SUM(U15:U21)</f>
-        <v>105</v>
-      </c>
-      <c r="V22" s="2">
-        <f>SUM(V15:V21)</f>
-        <v>48</v>
+      <c r="U23" s="2">
+        <f>SUM(U15:U22)</f>
+        <v>104</v>
+      </c>
+      <c r="V23" s="2">
+        <f>SUM(V15:V22)</f>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2081,7 +2133,7 @@
     <sortCondition ref="V3:V10"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:Q10 B15:Q21" xr:uid="{800ED500-2E94-4CC6-8AF0-CEB55BF076DD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:Q10 B15:Q22" xr:uid="{800ED500-2E94-4CC6-8AF0-CEB55BF076DD}">
       <formula1>"A,NA,DNP,L,W"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
week 4 after-match inputs
</commit_message>
<xml_diff>
--- a/data/Fall2022Schedule.xlsx
+++ b/data/Fall2022Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52193ECC-8576-413C-8C01-9B7F7E086074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D74D64-B079-4332-A18C-AC8C2F910C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="1350" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Wookie Mistakes" sheetId="2" r:id="rId1"/>
@@ -226,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -236,7 +236,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,7 +554,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G12" sqref="G12"/>
+      <selection pane="topRight" activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,67 +582,67 @@
         <v>27</v>
       </c>
       <c r="B2" s="1">
-        <v>44804</v>
+        <v>44803</v>
       </c>
       <c r="C2" s="1">
         <f t="shared" ref="C2:Q2" si="0">B2+7</f>
-        <v>44811</v>
+        <v>44810</v>
       </c>
       <c r="D2" s="1">
         <f t="shared" si="0"/>
-        <v>44818</v>
+        <v>44817</v>
       </c>
       <c r="E2" s="1">
         <f t="shared" si="0"/>
-        <v>44825</v>
+        <v>44824</v>
       </c>
       <c r="F2" s="1">
         <f t="shared" si="0"/>
-        <v>44832</v>
+        <v>44831</v>
       </c>
       <c r="G2" s="1">
         <f t="shared" si="0"/>
-        <v>44839</v>
+        <v>44838</v>
       </c>
       <c r="H2" s="1">
         <f t="shared" si="0"/>
-        <v>44846</v>
+        <v>44845</v>
       </c>
       <c r="I2" s="1">
         <f t="shared" si="0"/>
-        <v>44853</v>
+        <v>44852</v>
       </c>
       <c r="J2" s="1">
         <f t="shared" si="0"/>
-        <v>44860</v>
+        <v>44859</v>
       </c>
       <c r="K2" s="1">
         <f t="shared" si="0"/>
-        <v>44867</v>
+        <v>44866</v>
       </c>
       <c r="L2" s="1">
         <f t="shared" si="0"/>
-        <v>44874</v>
+        <v>44873</v>
       </c>
       <c r="M2" s="1">
         <f t="shared" si="0"/>
-        <v>44881</v>
+        <v>44880</v>
       </c>
       <c r="N2" s="1">
         <f t="shared" si="0"/>
-        <v>44888</v>
+        <v>44887</v>
       </c>
       <c r="O2" s="1">
         <f t="shared" si="0"/>
-        <v>44895</v>
+        <v>44894</v>
       </c>
       <c r="P2" s="1">
         <f t="shared" si="0"/>
-        <v>44902</v>
+        <v>44901</v>
       </c>
       <c r="Q2" s="1">
         <f t="shared" si="0"/>
-        <v>44909</v>
+        <v>44908</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>0</v>
@@ -678,7 +677,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
         <v>25</v>
@@ -690,7 +689,7 @@
         <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="J3" t="s">
         <v>25</v>
@@ -721,19 +720,19 @@
         <v>0.5</v>
       </c>
       <c r="S3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T10" si="2">S3-COUNTIF(B3:Q3, "W")-COUNTIF(B3:Q3, "L")</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U10" si="3">COUNTIF(B3:Q3, "A")</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V10" si="4">U3-T3</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="W3" t="s">
         <v>28</v>
@@ -753,7 +752,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
         <v>25</v>
@@ -765,7 +764,7 @@
         <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="J4" t="s">
         <v>25</v>
@@ -793,22 +792,22 @@
       </c>
       <c r="R4" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="S4">
         <v>6</v>
       </c>
       <c r="T4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U4">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="V4">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W4" t="s">
         <v>24</v>
@@ -828,7 +827,7 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
         <v>25</v>
@@ -840,7 +839,7 @@
         <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="J5" t="s">
         <v>25</v>
@@ -868,22 +867,22 @@
       </c>
       <c r="R5" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S5">
         <v>6</v>
       </c>
       <c r="T5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U5">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="V5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W5" t="s">
         <v>9</v>
@@ -903,7 +902,7 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
         <v>25</v>
@@ -915,7 +914,7 @@
         <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="J6" t="s">
         <v>25</v>
@@ -943,22 +942,22 @@
       </c>
       <c r="R6" s="6">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S6">
         <v>6</v>
       </c>
       <c r="T6">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="V6">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W6" t="s">
         <v>17</v>
@@ -978,7 +977,7 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
         <v>25</v>
@@ -990,7 +989,7 @@
         <v>25</v>
       </c>
       <c r="I7" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="J7" t="s">
         <v>25</v>
@@ -1025,15 +1024,15 @@
       </c>
       <c r="T7">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U7">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="V7">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W7" t="s">
         <v>20</v>
@@ -1053,7 +1052,7 @@
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
         <v>25</v>
@@ -1065,7 +1064,7 @@
         <v>25</v>
       </c>
       <c r="I8" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="J8" t="s">
         <v>25</v>
@@ -1104,11 +1103,11 @@
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="V8">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="W8" t="s">
         <v>15</v>
@@ -1128,7 +1127,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
         <v>25</v>
@@ -1140,7 +1139,7 @@
         <v>25</v>
       </c>
       <c r="I9" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="J9" t="s">
         <v>25</v>
@@ -1179,11 +1178,11 @@
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="V9">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="W9" t="s">
         <v>13</v>
@@ -1203,7 +1202,7 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
         <v>25</v>
@@ -1215,7 +1214,7 @@
         <v>25</v>
       </c>
       <c r="I10" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="J10" t="s">
         <v>25</v>
@@ -1243,22 +1242,22 @@
       </c>
       <c r="R10" s="6">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="S10">
         <v>6</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="V10">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W10" t="s">
         <v>22</v>
@@ -1280,9 +1279,9 @@
         <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
-      <c r="E11" s="5" t="e">
+      <c r="E11" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.8</v>
       </c>
       <c r="F11" s="5" t="e">
         <f t="shared" si="5"/>
@@ -1334,23 +1333,23 @@
       </c>
       <c r="R11" s="7">
         <f>AVERAGEIF(B11:O11, "&gt;=0")</f>
-        <v>0.6</v>
+        <v>0.64999999999999991</v>
       </c>
       <c r="S11" s="2">
         <f>SUM(S3:S10)</f>
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="T11" s="2">
         <f>SUM(T3:T10)</f>
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="U11" s="2">
         <f>SUM(U3:U10)</f>
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="V11" s="2">
         <f>SUM(V3:V10)</f>
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1358,67 +1357,67 @@
         <v>29</v>
       </c>
       <c r="B14" s="1">
-        <v>44804</v>
+        <v>44803</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" ref="C14:Q14" si="6">B14+7</f>
-        <v>44811</v>
+        <v>44810</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="6"/>
-        <v>44818</v>
+        <v>44817</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="6"/>
-        <v>44825</v>
+        <v>44824</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="6"/>
-        <v>44832</v>
+        <v>44831</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="6"/>
-        <v>44839</v>
+        <v>44838</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="6"/>
-        <v>44846</v>
+        <v>44845</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="6"/>
-        <v>44853</v>
+        <v>44852</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="6"/>
-        <v>44860</v>
+        <v>44859</v>
       </c>
       <c r="K14" s="1">
         <f t="shared" si="6"/>
-        <v>44867</v>
+        <v>44866</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="6"/>
-        <v>44874</v>
+        <v>44873</v>
       </c>
       <c r="M14" s="1">
         <f t="shared" si="6"/>
-        <v>44881</v>
+        <v>44880</v>
       </c>
       <c r="N14" s="1">
         <f t="shared" si="6"/>
-        <v>44888</v>
+        <v>44887</v>
       </c>
       <c r="O14" s="1">
         <f t="shared" si="6"/>
-        <v>44895</v>
+        <v>44894</v>
       </c>
       <c r="P14" s="1">
         <f t="shared" si="6"/>
-        <v>44902</v>
+        <v>44901</v>
       </c>
       <c r="Q14" s="1">
         <f t="shared" si="6"/>
-        <v>44909</v>
+        <v>44908</v>
       </c>
       <c r="R14" s="3" t="s">
         <v>0</v>
@@ -1453,7 +1452,7 @@
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
         <v>25</v>
@@ -1493,18 +1492,18 @@
       </c>
       <c r="R15" s="6">
         <f t="shared" ref="R15:R20" si="7">COUNTIF(B15:O15, "W")/(COUNTIF(B15:O15, "W")+COUNTIF(B15:O15, "L"))</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="S15">
         <v>10</v>
       </c>
       <c r="T15">
         <f t="shared" ref="T15:T20" si="8">S15-COUNTIF(B15:Q15, "W")-COUNTIF(B15:Q15, "L")</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U15">
         <f t="shared" ref="U15:U20" si="9">COUNTIF(B15:Q15, "A")</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V15">
         <f t="shared" ref="V15:V20" si="10">U15-T15</f>
@@ -1528,7 +1527,7 @@
         <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
         <v>25</v>
@@ -1575,11 +1574,11 @@
       </c>
       <c r="T16">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U16">
         <f t="shared" si="9"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V16">
         <f t="shared" si="10"/>
@@ -1603,7 +1602,7 @@
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s">
         <v>25</v>
@@ -1643,18 +1642,18 @@
       </c>
       <c r="R17" s="6">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S17">
         <v>10</v>
       </c>
       <c r="T17">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U17">
         <f t="shared" si="9"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V17">
         <f t="shared" si="10"/>
@@ -1678,7 +1677,7 @@
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
         <v>25</v>
@@ -1718,18 +1717,18 @@
       </c>
       <c r="R18" s="6">
         <f t="shared" si="7"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="S18">
         <v>10</v>
       </c>
       <c r="T18">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U18">
         <f t="shared" si="9"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V18">
         <f t="shared" si="10"/>
@@ -1753,7 +1752,7 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
         <v>25</v>
@@ -1804,11 +1803,11 @@
       </c>
       <c r="U19">
         <f t="shared" si="9"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V19">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W19" t="s">
         <v>22</v>
@@ -1828,7 +1827,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
         <v>25</v>
@@ -1879,11 +1878,11 @@
       </c>
       <c r="U20">
         <f t="shared" si="9"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V20">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W20" t="s">
         <v>33</v>
@@ -1903,7 +1902,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
         <v>25</v>
@@ -1954,18 +1953,18 @@
       </c>
       <c r="U21">
         <f>COUNTIF(B21:Q21, "A")</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V21">
         <f>U21-T21</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W21" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B22" t="s">
@@ -1978,7 +1977,7 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
         <v>25</v>
@@ -2018,18 +2017,18 @@
       </c>
       <c r="R22" s="6">
         <f>COUNTIF(B22:O22, "W")/(COUNTIF(B22:O22, "W")+COUNTIF(B22:O22, "L"))</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S22">
         <v>10</v>
       </c>
       <c r="T22">
         <f>S22-COUNTIF(B22:Q22, "W")-COUNTIF(B22:Q22, "L")</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U22">
         <f>COUNTIF(B22:Q22, "A")</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V22">
         <f>U22-T22</f>
@@ -2055,9 +2054,9 @@
         <f t="shared" si="11"/>
         <v>0.6</v>
       </c>
-      <c r="E23" s="5" t="e">
+      <c r="E23" s="5">
         <f t="shared" ref="E23" si="12">COUNTIF(E15:E22, "W")/(COUNTIF(E15:E22, "W")+COUNTIF(E15:E22, "L"))</f>
-        <v>#DIV/0!</v>
+        <v>0.8</v>
       </c>
       <c r="F23" s="5" t="e">
         <f t="shared" ref="F23" si="13">COUNTIF(F15:F22, "W")/(COUNTIF(F15:F22, "W")+COUNTIF(F15:F22, "L"))</f>
@@ -2109,7 +2108,7 @@
       </c>
       <c r="R23" s="7">
         <f>AVERAGEIF(B23:O23, "&gt;=0")</f>
-        <v>0.53333333333333333</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="S23" s="2">
         <f>SUM(S15:S22)</f>
@@ -2117,15 +2116,15 @@
       </c>
       <c r="T23" s="2">
         <f>SUM(T15:T22)</f>
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="U23" s="2">
         <f>SUM(U15:U22)</f>
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="V23" s="2">
         <f>SUM(V15:V22)</f>
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2133,7 +2132,7 @@
     <sortCondition ref="V3:V10"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:Q10 B15:Q22" xr:uid="{800ED500-2E94-4CC6-8AF0-CEB55BF076DD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:Q22 B3:Q10" xr:uid="{800ED500-2E94-4CC6-8AF0-CEB55BF076DD}">
       <formula1>"A,NA,DNP,L,W"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
all fall 22 week 6 inputs complete
</commit_message>
<xml_diff>
--- a/data/Fall2022Schedule.xlsx
+++ b/data/Fall2022Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D74D64-B079-4332-A18C-AC8C2F910C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3703A86-C7C2-4AC9-A304-2AE29152E771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
   </bookViews>
@@ -554,7 +554,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T5" sqref="T5"/>
+      <selection pane="topRight" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,10 +680,10 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
         <v>25</v>
@@ -717,18 +717,18 @@
       </c>
       <c r="R3" s="6">
         <f t="shared" ref="R3:R10" si="1">COUNTIF(B3:O3, "W")/(COUNTIF(B3:O3, "W")+COUNTIF(B3:O3, "L"))</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="S3">
         <v>6</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T10" si="2">S3-COUNTIF(B3:Q3, "W")-COUNTIF(B3:Q3, "L")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U10" si="3">COUNTIF(B3:Q3, "A")</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V10" si="4">U3-T3</f>
@@ -755,10 +755,10 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
         <v>25</v>
@@ -792,18 +792,18 @@
       </c>
       <c r="R4" s="6">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.6</v>
       </c>
       <c r="S4">
         <v>6</v>
       </c>
       <c r="T4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U4">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="V4">
         <f t="shared" si="4"/>
@@ -830,10 +830,10 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
         <v>25</v>
@@ -867,18 +867,18 @@
       </c>
       <c r="R5" s="6">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="S5">
         <v>6</v>
       </c>
       <c r="T5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U5">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="V5">
         <f t="shared" si="4"/>
@@ -905,10 +905,10 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
         <v>25</v>
@@ -942,22 +942,22 @@
       </c>
       <c r="R6" s="6">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="S6">
         <v>6</v>
       </c>
       <c r="T6">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="V6">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W6" t="s">
         <v>17</v>
@@ -980,10 +980,10 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
         <v>25</v>
@@ -1017,22 +1017,22 @@
       </c>
       <c r="R7" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="S7">
         <v>6</v>
       </c>
       <c r="T7">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U7">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="V7">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W7" t="s">
         <v>20</v>
@@ -1055,10 +1055,10 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="H8" t="s">
         <v>25</v>
@@ -1099,15 +1099,15 @@
       </c>
       <c r="T8">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="V8">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W8" t="s">
         <v>15</v>
@@ -1130,10 +1130,10 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
         <v>25</v>
@@ -1174,15 +1174,15 @@
       </c>
       <c r="T9">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="V9">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W9" t="s">
         <v>13</v>
@@ -1205,10 +1205,10 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="H10" t="s">
         <v>25</v>
@@ -1253,11 +1253,11 @@
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="V10">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="W10" t="s">
         <v>22</v>
@@ -1283,13 +1283,13 @@
         <f t="shared" si="5"/>
         <v>0.8</v>
       </c>
-      <c r="F11" s="5" t="e">
+      <c r="F11" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G11" s="5" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="G11" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="H11" s="5" t="e">
         <f t="shared" si="5"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="R11" s="7">
         <f>AVERAGEIF(B11:O11, "&gt;=0")</f>
-        <v>0.64999999999999991</v>
+        <v>0.73333333333333328</v>
       </c>
       <c r="S11" s="2">
         <f>SUM(S3:S10)</f>
@@ -1341,15 +1341,15 @@
       </c>
       <c r="T11" s="2">
         <f>SUM(T3:T10)</f>
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="U11" s="2">
         <f>SUM(U3:U10)</f>
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="V11" s="2">
         <f>SUM(V3:V10)</f>
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1455,10 +1455,10 @@
         <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="H15" t="s">
         <v>25</v>
@@ -1492,22 +1492,22 @@
       </c>
       <c r="R15" s="6">
         <f t="shared" ref="R15:R20" si="7">COUNTIF(B15:O15, "W")/(COUNTIF(B15:O15, "W")+COUNTIF(B15:O15, "L"))</f>
-        <v>0.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="S15">
         <v>10</v>
       </c>
       <c r="T15">
         <f t="shared" ref="T15:T20" si="8">S15-COUNTIF(B15:Q15, "W")-COUNTIF(B15:Q15, "L")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U15">
         <f t="shared" ref="U15:U20" si="9">COUNTIF(B15:Q15, "A")</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V15">
         <f t="shared" ref="V15:V20" si="10">U15-T15</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W15" t="s">
         <v>13</v>
@@ -1530,10 +1530,10 @@
         <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="H16" t="s">
         <v>25</v>
@@ -1567,22 +1567,22 @@
       </c>
       <c r="R16" s="6">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="S16">
         <v>10</v>
       </c>
       <c r="T16">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U16">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V16">
         <f t="shared" si="10"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W16" t="s">
         <v>15</v>
@@ -1605,10 +1605,10 @@
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
         <v>25</v>
@@ -1642,18 +1642,18 @@
       </c>
       <c r="R17" s="6">
         <f t="shared" si="7"/>
-        <v>0.66666666666666663</v>
+        <v>0.6</v>
       </c>
       <c r="S17">
         <v>10</v>
       </c>
       <c r="T17">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="U17">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V17">
         <f t="shared" si="10"/>
@@ -1680,10 +1680,10 @@
         <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="H18" t="s">
         <v>25</v>
@@ -1717,22 +1717,22 @@
       </c>
       <c r="R18" s="6">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S18">
         <v>10</v>
       </c>
       <c r="T18">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U18">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V18">
         <f t="shared" si="10"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W18" t="s">
         <v>20</v>
@@ -1755,10 +1755,10 @@
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
         <v>25</v>
@@ -1792,18 +1792,18 @@
       </c>
       <c r="R19" s="6">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S19">
         <v>10</v>
       </c>
       <c r="T19">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="U19">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V19">
         <f t="shared" si="10"/>
@@ -1830,10 +1830,10 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="H20" t="s">
         <v>25</v>
@@ -1867,22 +1867,22 @@
       </c>
       <c r="R20" s="6">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S20">
         <v>6</v>
       </c>
       <c r="T20">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U20">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V20">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W20" t="s">
         <v>33</v>
@@ -1905,10 +1905,10 @@
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="H21" t="s">
         <v>25</v>
@@ -1953,11 +1953,11 @@
       </c>
       <c r="U21">
         <f>COUNTIF(B21:Q21, "A")</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V21">
         <f>U21-T21</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="W21" t="s">
         <v>32</v>
@@ -1980,10 +1980,10 @@
         <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="H22" t="s">
         <v>25</v>
@@ -2024,11 +2024,11 @@
       </c>
       <c r="T22">
         <f>S22-COUNTIF(B22:Q22, "W")-COUNTIF(B22:Q22, "L")</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="U22">
         <f>COUNTIF(B22:Q22, "A")</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V22">
         <f>U22-T22</f>
@@ -2058,13 +2058,13 @@
         <f t="shared" ref="E23" si="12">COUNTIF(E15:E22, "W")/(COUNTIF(E15:E22, "W")+COUNTIF(E15:E22, "L"))</f>
         <v>0.8</v>
       </c>
-      <c r="F23" s="5" t="e">
+      <c r="F23" s="5">
         <f t="shared" ref="F23" si="13">COUNTIF(F15:F22, "W")/(COUNTIF(F15:F22, "W")+COUNTIF(F15:F22, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G23" s="5" t="e">
+        <v>0.4</v>
+      </c>
+      <c r="G23" s="5">
         <f t="shared" ref="G23" si="14">COUNTIF(G15:G22, "W")/(COUNTIF(G15:G22, "W")+COUNTIF(G15:G22, "L"))</f>
-        <v>#DIV/0!</v>
+        <v>0.4</v>
       </c>
       <c r="H23" s="5" t="e">
         <f t="shared" ref="H23" si="15">COUNTIF(H15:H22, "W")/(COUNTIF(H15:H22, "W")+COUNTIF(H15:H22, "L"))</f>
@@ -2108,7 +2108,7 @@
       </c>
       <c r="R23" s="7">
         <f>AVERAGEIF(B23:O23, "&gt;=0")</f>
-        <v>0.60000000000000009</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="S23" s="2">
         <f>SUM(S15:S22)</f>
@@ -2116,15 +2116,15 @@
       </c>
       <c r="T23" s="2">
         <f>SUM(T15:T22)</f>
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="U23" s="2">
         <f>SUM(U15:U22)</f>
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="V23" s="2">
         <f>SUM(V15:V22)</f>
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall 22 week 7 complete
</commit_message>
<xml_diff>
--- a/data/Fall2022Schedule.xlsx
+++ b/data/Fall2022Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3703A86-C7C2-4AC9-A304-2AE29152E771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414F4C1F-599E-4933-8AAA-FE1842112410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
+    <workbookView xWindow="19335" yWindow="2400" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Wookie Mistakes" sheetId="2" r:id="rId1"/>
@@ -554,7 +554,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K28" sqref="K28"/>
+      <selection pane="topRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,7 +686,7 @@
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
         <v>10</v>
@@ -728,11 +728,11 @@
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U10" si="3">COUNTIF(B3:Q3, "A")</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V10" si="4">U3-T3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W3" t="s">
         <v>28</v>
@@ -761,7 +761,7 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
@@ -792,18 +792,18 @@
       </c>
       <c r="R4" s="6">
         <f t="shared" si="1"/>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="S4">
         <v>6</v>
       </c>
       <c r="T4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V4">
         <f t="shared" si="4"/>
@@ -836,7 +836,7 @@
         <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="I5" t="s">
         <v>10</v>
@@ -867,18 +867,18 @@
       </c>
       <c r="R5" s="6">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="S5">
         <v>6</v>
       </c>
       <c r="T5">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U5">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V5">
         <f t="shared" si="4"/>
@@ -911,7 +911,7 @@
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
@@ -953,11 +953,11 @@
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V6">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W6" t="s">
         <v>17</v>
@@ -986,7 +986,7 @@
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="I7" t="s">
         <v>10</v>
@@ -1017,18 +1017,18 @@
       </c>
       <c r="R7" s="6">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="S7">
         <v>6</v>
       </c>
       <c r="T7">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U7">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V7">
         <f t="shared" si="4"/>
@@ -1061,7 +1061,7 @@
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="I8" t="s">
         <v>10</v>
@@ -1099,11 +1099,11 @@
       </c>
       <c r="T8">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V8">
         <f t="shared" si="4"/>
@@ -1136,7 +1136,7 @@
         <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="I9" t="s">
         <v>10</v>
@@ -1178,11 +1178,11 @@
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V9">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W9" t="s">
         <v>13</v>
@@ -1211,7 +1211,7 @@
         <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="I10" t="s">
         <v>10</v>
@@ -1242,18 +1242,18 @@
       </c>
       <c r="R10" s="6">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S10">
         <v>6</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V10">
         <f t="shared" si="4"/>
@@ -1291,9 +1291,9 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="H11" s="5" t="e">
+      <c r="H11" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.4</v>
       </c>
       <c r="I11" s="5" t="e">
         <f t="shared" si="5"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="R11" s="7">
         <f>AVERAGEIF(B11:O11, "&gt;=0")</f>
-        <v>0.73333333333333328</v>
+        <v>0.68571428571428572</v>
       </c>
       <c r="S11" s="2">
         <f>SUM(S3:S10)</f>
@@ -1341,15 +1341,15 @@
       </c>
       <c r="T11" s="2">
         <f>SUM(T3:T10)</f>
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="U11" s="2">
         <f>SUM(U3:U10)</f>
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="V11" s="2">
         <f>SUM(V3:V10)</f>
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1461,10 +1461,10 @@
         <v>7</v>
       </c>
       <c r="H15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="I15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="J15" t="s">
         <v>25</v>
@@ -1492,18 +1492,18 @@
       </c>
       <c r="R15" s="6">
         <f t="shared" ref="R15:R20" si="7">COUNTIF(B15:O15, "W")/(COUNTIF(B15:O15, "W")+COUNTIF(B15:O15, "L"))</f>
-        <v>0.33333333333333331</v>
+        <v>0.6</v>
       </c>
       <c r="S15">
         <v>10</v>
       </c>
       <c r="T15">
         <f t="shared" ref="T15:T20" si="8">S15-COUNTIF(B15:Q15, "W")-COUNTIF(B15:Q15, "L")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="U15">
         <f t="shared" ref="U15:U20" si="9">COUNTIF(B15:Q15, "A")</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V15">
         <f t="shared" ref="V15:V20" si="10">U15-T15</f>
@@ -1536,10 +1536,10 @@
         <v>10</v>
       </c>
       <c r="H16" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="I16" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="J16" t="s">
         <v>25</v>
@@ -1567,22 +1567,22 @@
       </c>
       <c r="R16" s="6">
         <f t="shared" si="7"/>
-        <v>0.8</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S16">
         <v>10</v>
       </c>
       <c r="T16">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U16">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V16">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W16" t="s">
         <v>15</v>
@@ -1611,10 +1611,10 @@
         <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="I17" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="J17" t="s">
         <v>25</v>
@@ -1642,22 +1642,22 @@
       </c>
       <c r="R17" s="6">
         <f t="shared" si="7"/>
-        <v>0.6</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S17">
         <v>10</v>
       </c>
       <c r="T17">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U17">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V17">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W17" t="s">
         <v>28</v>
@@ -1686,10 +1686,10 @@
         <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="I18" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="J18" t="s">
         <v>25</v>
@@ -1728,11 +1728,11 @@
       </c>
       <c r="U18">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V18">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="W18" t="s">
         <v>20</v>
@@ -1761,10 +1761,10 @@
         <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="I19" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="J19" t="s">
         <v>25</v>
@@ -1792,22 +1792,22 @@
       </c>
       <c r="R19" s="6">
         <f t="shared" si="7"/>
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="S19">
         <v>10</v>
       </c>
       <c r="T19">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U19">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V19">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W19" t="s">
         <v>22</v>
@@ -1836,10 +1836,10 @@
         <v>8</v>
       </c>
       <c r="H20" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="J20" t="s">
         <v>25</v>
@@ -1867,22 +1867,22 @@
       </c>
       <c r="R20" s="6">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S20">
         <v>6</v>
       </c>
       <c r="T20">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U20">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V20">
         <f t="shared" si="10"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W20" t="s">
         <v>33</v>
@@ -1911,10 +1911,10 @@
         <v>10</v>
       </c>
       <c r="H21" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="I21" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="J21" t="s">
         <v>25</v>
@@ -1942,18 +1942,18 @@
       </c>
       <c r="R21" s="6">
         <f>COUNTIF(B21:O21, "W")/(COUNTIF(B21:O21, "W")+COUNTIF(B21:O21, "L"))</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="S21">
         <v>6</v>
       </c>
       <c r="T21">
         <f>S21-COUNTIF(B21:Q21, "W")-COUNTIF(B21:Q21, "L")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U21">
         <f>COUNTIF(B21:Q21, "A")</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V21">
         <f>U21-T21</f>
@@ -1986,10 +1986,10 @@
         <v>7</v>
       </c>
       <c r="H22" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="I22" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="J22" t="s">
         <v>25</v>
@@ -2017,18 +2017,18 @@
       </c>
       <c r="R22" s="6">
         <f>COUNTIF(B22:O22, "W")/(COUNTIF(B22:O22, "W")+COUNTIF(B22:O22, "L"))</f>
-        <v>0.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="S22">
         <v>10</v>
       </c>
       <c r="T22">
         <f>S22-COUNTIF(B22:Q22, "W")-COUNTIF(B22:Q22, "L")</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U22">
         <f>COUNTIF(B22:Q22, "A")</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V22">
         <f>U22-T22</f>
@@ -2066,13 +2066,13 @@
         <f t="shared" ref="G23" si="14">COUNTIF(G15:G22, "W")/(COUNTIF(G15:G22, "W")+COUNTIF(G15:G22, "L"))</f>
         <v>0.4</v>
       </c>
-      <c r="H23" s="5" t="e">
+      <c r="H23" s="5">
         <f t="shared" ref="H23" si="15">COUNTIF(H15:H22, "W")/(COUNTIF(H15:H22, "W")+COUNTIF(H15:H22, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I23" s="5" t="e">
+        <v>0.6</v>
+      </c>
+      <c r="I23" s="5">
         <f t="shared" ref="I23" si="16">COUNTIF(I15:I22, "W")/(COUNTIF(I15:I22, "W")+COUNTIF(I15:I22, "L"))</f>
-        <v>#DIV/0!</v>
+        <v>0.6</v>
       </c>
       <c r="J23" s="5" t="e">
         <f t="shared" ref="J23" si="17">COUNTIF(J15:J22, "W")/(COUNTIF(J15:J22, "W")+COUNTIF(J15:J22, "L"))</f>
@@ -2108,7 +2108,7 @@
       </c>
       <c r="R23" s="7">
         <f>AVERAGEIF(B23:O23, "&gt;=0")</f>
-        <v>0.53333333333333333</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S23" s="2">
         <f>SUM(S15:S22)</f>
@@ -2116,15 +2116,15 @@
       </c>
       <c r="T23" s="2">
         <f>SUM(T15:T22)</f>
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="U23" s="2">
         <f>SUM(U15:U22)</f>
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="V23" s="2">
         <f>SUM(V15:V22)</f>
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall 22 week 9 day after commits
</commit_message>
<xml_diff>
--- a/data/Fall2022Schedule.xlsx
+++ b/data/Fall2022Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414F4C1F-599E-4933-8AAA-FE1842112410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F47472-7866-41CD-8820-B5EE1B023483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19335" yWindow="2400" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
+    <workbookView xWindow="2805" yWindow="2160" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Wookie Mistakes" sheetId="2" r:id="rId1"/>
@@ -552,9 +552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA30A97-9145-4EDA-8DB9-44B6A1233BAB}">
   <dimension ref="A2:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J17" sqref="J17"/>
+      <selection pane="topRight" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +692,7 @@
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="K3" t="s">
         <v>25</v>
@@ -728,11 +728,11 @@
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U10" si="3">COUNTIF(B3:Q3, "A")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V10" si="4">U3-T3</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W3" t="s">
         <v>28</v>
@@ -767,7 +767,7 @@
         <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="K4" t="s">
         <v>25</v>
@@ -792,18 +792,18 @@
       </c>
       <c r="R4" s="6">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="S4">
         <v>6</v>
       </c>
       <c r="T4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="U4">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V4">
         <f t="shared" si="4"/>
@@ -842,7 +842,7 @@
         <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="K5" t="s">
         <v>25</v>
@@ -878,11 +878,11 @@
       </c>
       <c r="U5">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V5">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W5" t="s">
         <v>9</v>
@@ -917,7 +917,7 @@
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="K6" t="s">
         <v>25</v>
@@ -942,18 +942,18 @@
       </c>
       <c r="R6" s="6">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="S6">
         <v>6</v>
       </c>
       <c r="T6">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V6">
         <f t="shared" si="4"/>
@@ -992,7 +992,7 @@
         <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="K7" t="s">
         <v>25</v>
@@ -1028,11 +1028,11 @@
       </c>
       <c r="U7">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V7">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W7" t="s">
         <v>20</v>
@@ -1067,7 +1067,7 @@
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="K8" t="s">
         <v>25</v>
@@ -1092,18 +1092,18 @@
       </c>
       <c r="R8" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="S8">
         <v>6</v>
       </c>
       <c r="T8">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V8">
         <f t="shared" si="4"/>
@@ -1142,7 +1142,7 @@
         <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="K9" t="s">
         <v>25</v>
@@ -1167,18 +1167,18 @@
       </c>
       <c r="R9" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S9">
         <v>6</v>
       </c>
       <c r="T9">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V9">
         <f t="shared" si="4"/>
@@ -1217,7 +1217,7 @@
         <v>10</v>
       </c>
       <c r="J10" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="K10" t="s">
         <v>25</v>
@@ -1253,11 +1253,11 @@
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V10">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W10" t="s">
         <v>22</v>
@@ -1299,9 +1299,9 @@
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J11" s="5" t="e">
+      <c r="J11" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.5</v>
       </c>
       <c r="K11" s="5" t="e">
         <f t="shared" si="5"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="R11" s="7">
         <f>AVERAGEIF(B11:O11, "&gt;=0")</f>
-        <v>0.68571428571428572</v>
+        <v>0.66249999999999998</v>
       </c>
       <c r="S11" s="2">
         <f>SUM(S3:S10)</f>
@@ -1341,15 +1341,15 @@
       </c>
       <c r="T11" s="2">
         <f>SUM(T3:T10)</f>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="U11" s="2">
         <f>SUM(U3:U10)</f>
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="V11" s="2">
         <f>SUM(V3:V10)</f>
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1467,7 +1467,7 @@
         <v>12</v>
       </c>
       <c r="J15" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="K15" t="s">
         <v>25</v>
@@ -1492,18 +1492,18 @@
       </c>
       <c r="R15" s="6">
         <f t="shared" ref="R15:R20" si="7">COUNTIF(B15:O15, "W")/(COUNTIF(B15:O15, "W")+COUNTIF(B15:O15, "L"))</f>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="S15">
         <v>10</v>
       </c>
       <c r="T15">
         <f t="shared" ref="T15:T20" si="8">S15-COUNTIF(B15:Q15, "W")-COUNTIF(B15:Q15, "L")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U15">
         <f t="shared" ref="U15:U20" si="9">COUNTIF(B15:Q15, "A")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V15">
         <f t="shared" ref="V15:V20" si="10">U15-T15</f>
@@ -1542,7 +1542,7 @@
         <v>7</v>
       </c>
       <c r="J16" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="K16" t="s">
         <v>25</v>
@@ -1578,11 +1578,11 @@
       </c>
       <c r="U16">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V16">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W16" t="s">
         <v>15</v>
@@ -1617,7 +1617,7 @@
         <v>8</v>
       </c>
       <c r="J17" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="K17" t="s">
         <v>25</v>
@@ -1642,18 +1642,18 @@
       </c>
       <c r="R17" s="6">
         <f t="shared" si="7"/>
-        <v>0.66666666666666663</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="S17">
         <v>10</v>
       </c>
       <c r="T17">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U17">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V17">
         <f t="shared" si="10"/>
@@ -1692,7 +1692,7 @@
         <v>8</v>
       </c>
       <c r="J18" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="K18" t="s">
         <v>25</v>
@@ -1717,18 +1717,18 @@
       </c>
       <c r="R18" s="6">
         <f t="shared" si="7"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="S18">
         <v>10</v>
       </c>
       <c r="T18">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U18">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V18">
         <f t="shared" si="10"/>
@@ -1767,7 +1767,7 @@
         <v>8</v>
       </c>
       <c r="J19" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="K19" t="s">
         <v>25</v>
@@ -1792,18 +1792,18 @@
       </c>
       <c r="R19" s="6">
         <f t="shared" si="7"/>
-        <v>0.4</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="S19">
         <v>10</v>
       </c>
       <c r="T19">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U19">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V19">
         <f t="shared" si="10"/>
@@ -1842,7 +1842,7 @@
         <v>12</v>
       </c>
       <c r="J20" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="K20" t="s">
         <v>25</v>
@@ -1878,11 +1878,11 @@
       </c>
       <c r="U20">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V20">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W20" t="s">
         <v>33</v>
@@ -1917,7 +1917,7 @@
         <v>12</v>
       </c>
       <c r="J21" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="K21" t="s">
         <v>25</v>
@@ -1953,11 +1953,11 @@
       </c>
       <c r="U21">
         <f>COUNTIF(B21:Q21, "A")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V21">
         <f>U21-T21</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W21" t="s">
         <v>32</v>
@@ -1992,7 +1992,7 @@
         <v>7</v>
       </c>
       <c r="J22" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="K22" t="s">
         <v>25</v>
@@ -2017,18 +2017,18 @@
       </c>
       <c r="R22" s="6">
         <f>COUNTIF(B22:O22, "W")/(COUNTIF(B22:O22, "W")+COUNTIF(B22:O22, "L"))</f>
-        <v>0.33333333333333331</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="S22">
         <v>10</v>
       </c>
       <c r="T22">
         <f>S22-COUNTIF(B22:Q22, "W")-COUNTIF(B22:Q22, "L")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U22">
         <f>COUNTIF(B22:Q22, "A")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V22">
         <f>U22-T22</f>
@@ -2074,9 +2074,9 @@
         <f t="shared" ref="I23" si="16">COUNTIF(I15:I22, "W")/(COUNTIF(I15:I22, "W")+COUNTIF(I15:I22, "L"))</f>
         <v>0.6</v>
       </c>
-      <c r="J23" s="5" t="e">
+      <c r="J23" s="5">
         <f t="shared" ref="J23" si="17">COUNTIF(J15:J22, "W")/(COUNTIF(J15:J22, "W")+COUNTIF(J15:J22, "L"))</f>
-        <v>#DIV/0!</v>
+        <v>0.6</v>
       </c>
       <c r="K23" s="5" t="e">
         <f t="shared" ref="K23" si="18">COUNTIF(K15:K22, "W")/(COUNTIF(K15:K22, "W")+COUNTIF(K15:K22, "L"))</f>
@@ -2108,7 +2108,7 @@
       </c>
       <c r="R23" s="7">
         <f>AVERAGEIF(B23:O23, "&gt;=0")</f>
-        <v>0.55000000000000004</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="S23" s="2">
         <f>SUM(S15:S22)</f>
@@ -2116,15 +2116,15 @@
       </c>
       <c r="T23" s="2">
         <f>SUM(T15:T22)</f>
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="U23" s="2">
         <f>SUM(U15:U22)</f>
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="V23" s="2">
         <f>SUM(V15:V22)</f>
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall 22 week 10 day-after inputs
</commit_message>
<xml_diff>
--- a/data/Fall2022Schedule.xlsx
+++ b/data/Fall2022Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F47472-7866-41CD-8820-B5EE1B023483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98303FA2-6E4C-42E2-B090-9299D4761600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="2160" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
+    <workbookView xWindow="18435" yWindow="2025" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Wookie Mistakes" sheetId="2" r:id="rId1"/>
@@ -552,9 +552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA30A97-9145-4EDA-8DB9-44B6A1233BAB}">
   <dimension ref="A2:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K18" sqref="K18"/>
+      <selection pane="topRight" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +695,7 @@
         <v>10</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L3" t="s">
         <v>25</v>
@@ -717,18 +717,18 @@
       </c>
       <c r="R3" s="6">
         <f t="shared" ref="R3:R10" si="1">COUNTIF(B3:O3, "W")/(COUNTIF(B3:O3, "W")+COUNTIF(B3:O3, "L"))</f>
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="S3">
         <v>6</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T10" si="2">S3-COUNTIF(B3:Q3, "W")-COUNTIF(B3:Q3, "L")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U10" si="3">COUNTIF(B3:Q3, "A")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V10" si="4">U3-T3</f>
@@ -770,7 +770,7 @@
         <v>12</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="L4" t="s">
         <v>25</v>
@@ -803,11 +803,11 @@
       </c>
       <c r="U4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W4" t="s">
         <v>24</v>
@@ -845,7 +845,7 @@
         <v>8</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L5" t="s">
         <v>25</v>
@@ -867,18 +867,18 @@
       </c>
       <c r="R5" s="6">
         <f t="shared" si="1"/>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="S5">
         <v>6</v>
       </c>
       <c r="T5">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V5">
         <f t="shared" si="4"/>
@@ -920,7 +920,7 @@
         <v>12</v>
       </c>
       <c r="K6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="L6" t="s">
         <v>25</v>
@@ -953,11 +953,11 @@
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V6">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W6" t="s">
         <v>17</v>
@@ -995,7 +995,7 @@
         <v>10</v>
       </c>
       <c r="K7" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L7" t="s">
         <v>25</v>
@@ -1017,18 +1017,18 @@
       </c>
       <c r="R7" s="6">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S7">
         <v>6</v>
       </c>
       <c r="T7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V7">
         <f t="shared" si="4"/>
@@ -1070,7 +1070,7 @@
         <v>7</v>
       </c>
       <c r="K8" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="L8" t="s">
         <v>25</v>
@@ -1103,11 +1103,11 @@
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V8">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W8" t="s">
         <v>15</v>
@@ -1145,7 +1145,7 @@
         <v>7</v>
       </c>
       <c r="K9" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="L9" t="s">
         <v>25</v>
@@ -1167,18 +1167,18 @@
       </c>
       <c r="R9" s="6">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="S9">
         <v>6</v>
       </c>
       <c r="T9">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V9">
         <f t="shared" si="4"/>
@@ -1220,7 +1220,7 @@
         <v>10</v>
       </c>
       <c r="K10" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="L10" t="s">
         <v>25</v>
@@ -1242,18 +1242,18 @@
       </c>
       <c r="R10" s="6">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="S10">
         <v>6</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V10">
         <f t="shared" si="4"/>
@@ -1303,9 +1303,9 @@
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="K11" s="5" t="e">
+      <c r="K11" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.4</v>
       </c>
       <c r="L11" s="5" t="e">
         <f t="shared" si="5"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="R11" s="7">
         <f>AVERAGEIF(B11:O11, "&gt;=0")</f>
-        <v>0.66249999999999998</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="S11" s="2">
         <f>SUM(S3:S10)</f>
@@ -1341,15 +1341,15 @@
       </c>
       <c r="T11" s="2">
         <f>SUM(T3:T10)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="U11" s="2">
         <f>SUM(U3:U10)</f>
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="V11" s="2">
         <f>SUM(V3:V10)</f>
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1470,7 +1470,7 @@
         <v>7</v>
       </c>
       <c r="K15" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L15" t="s">
         <v>25</v>
@@ -1492,18 +1492,18 @@
       </c>
       <c r="R15" s="6">
         <f t="shared" ref="R15:R20" si="7">COUNTIF(B15:O15, "W")/(COUNTIF(B15:O15, "W")+COUNTIF(B15:O15, "L"))</f>
-        <v>0.5</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="S15">
         <v>10</v>
       </c>
       <c r="T15">
         <f t="shared" ref="T15:T20" si="8">S15-COUNTIF(B15:Q15, "W")-COUNTIF(B15:Q15, "L")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U15">
         <f t="shared" ref="U15:U20" si="9">COUNTIF(B15:Q15, "A")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V15">
         <f t="shared" ref="V15:V20" si="10">U15-T15</f>
@@ -1545,7 +1545,7 @@
         <v>10</v>
       </c>
       <c r="K16" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L16" t="s">
         <v>25</v>
@@ -1567,18 +1567,18 @@
       </c>
       <c r="R16" s="6">
         <f t="shared" si="7"/>
-        <v>0.66666666666666663</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="S16">
         <v>10</v>
       </c>
       <c r="T16">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U16">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V16">
         <f t="shared" si="10"/>
@@ -1620,7 +1620,7 @@
         <v>12</v>
       </c>
       <c r="K17" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="L17" t="s">
         <v>25</v>
@@ -1653,11 +1653,11 @@
       </c>
       <c r="U17">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V17">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W17" t="s">
         <v>28</v>
@@ -1695,7 +1695,7 @@
         <v>12</v>
       </c>
       <c r="K18" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="L18" t="s">
         <v>25</v>
@@ -1717,18 +1717,18 @@
       </c>
       <c r="R18" s="6">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="S18">
         <v>10</v>
       </c>
       <c r="T18">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U18">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V18">
         <f t="shared" si="10"/>
@@ -1770,7 +1770,7 @@
         <v>7</v>
       </c>
       <c r="K19" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L19" t="s">
         <v>25</v>
@@ -1792,18 +1792,18 @@
       </c>
       <c r="R19" s="6">
         <f t="shared" si="7"/>
-        <v>0.33333333333333331</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="S19">
         <v>10</v>
       </c>
       <c r="T19">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U19">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V19">
         <f t="shared" si="10"/>
@@ -1845,7 +1845,7 @@
         <v>10</v>
       </c>
       <c r="K20" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="L20" t="s">
         <v>25</v>
@@ -1867,18 +1867,18 @@
       </c>
       <c r="R20" s="6">
         <f t="shared" si="7"/>
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="S20">
         <v>6</v>
       </c>
       <c r="T20">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U20">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V20">
         <f t="shared" si="10"/>
@@ -1920,7 +1920,7 @@
         <v>10</v>
       </c>
       <c r="K21" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="L21" t="s">
         <v>25</v>
@@ -1953,11 +1953,11 @@
       </c>
       <c r="U21">
         <f>COUNTIF(B21:Q21, "A")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V21">
         <f>U21-T21</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W21" t="s">
         <v>32</v>
@@ -1995,7 +1995,7 @@
         <v>12</v>
       </c>
       <c r="K22" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="L22" t="s">
         <v>25</v>
@@ -2028,11 +2028,11 @@
       </c>
       <c r="U22">
         <f>COUNTIF(B22:Q22, "A")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V22">
         <f>U22-T22</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W22" t="s">
         <v>35</v>
@@ -2078,9 +2078,9 @@
         <f t="shared" ref="J23" si="17">COUNTIF(J15:J22, "W")/(COUNTIF(J15:J22, "W")+COUNTIF(J15:J22, "L"))</f>
         <v>0.6</v>
       </c>
-      <c r="K23" s="5" t="e">
+      <c r="K23" s="5">
         <f t="shared" ref="K23" si="18">COUNTIF(K15:K22, "W")/(COUNTIF(K15:K22, "W")+COUNTIF(K15:K22, "L"))</f>
-        <v>#DIV/0!</v>
+        <v>0.4</v>
       </c>
       <c r="L23" s="5" t="e">
         <f t="shared" ref="L23" si="19">COUNTIF(L15:L22, "W")/(COUNTIF(L15:L22, "W")+COUNTIF(L15:L22, "L"))</f>
@@ -2108,7 +2108,7 @@
       </c>
       <c r="R23" s="7">
         <f>AVERAGEIF(B23:O23, "&gt;=0")</f>
-        <v>0.55555555555555558</v>
+        <v>0.54</v>
       </c>
       <c r="S23" s="2">
         <f>SUM(S15:S22)</f>
@@ -2116,15 +2116,15 @@
       </c>
       <c r="T23" s="2">
         <f>SUM(T15:T22)</f>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="U23" s="2">
         <f>SUM(U15:U22)</f>
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="V23" s="2">
         <f>SUM(V15:V22)</f>
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall 22 week 11 day-after inputs
</commit_message>
<xml_diff>
--- a/data/Fall2022Schedule.xlsx
+++ b/data/Fall2022Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98303FA2-6E4C-42E2-B090-9299D4761600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B5F007-F3A6-4B37-9E76-DEB32C2DB08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18435" yWindow="2025" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
   </bookViews>
@@ -554,7 +554,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K25" sqref="K25"/>
+      <selection pane="topRight" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +698,7 @@
         <v>7</v>
       </c>
       <c r="L3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="M3" t="s">
         <v>25</v>
@@ -717,18 +717,18 @@
       </c>
       <c r="R3" s="6">
         <f t="shared" ref="R3:R10" si="1">COUNTIF(B3:O3, "W")/(COUNTIF(B3:O3, "W")+COUNTIF(B3:O3, "L"))</f>
-        <v>0.6</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S3">
         <v>6</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T10" si="2">S3-COUNTIF(B3:Q3, "W")-COUNTIF(B3:Q3, "L")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U10" si="3">COUNTIF(B3:Q3, "A")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V10" si="4">U3-T3</f>
@@ -773,7 +773,7 @@
         <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="M4" t="s">
         <v>25</v>
@@ -792,18 +792,18 @@
       </c>
       <c r="R4" s="6">
         <f t="shared" si="1"/>
-        <v>0.5714285714285714</v>
+        <v>0.625</v>
       </c>
       <c r="S4">
         <v>6</v>
       </c>
       <c r="T4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="U4">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V4">
         <f t="shared" si="4"/>
@@ -848,7 +848,7 @@
         <v>7</v>
       </c>
       <c r="L5" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="M5" t="s">
         <v>25</v>
@@ -878,11 +878,11 @@
       </c>
       <c r="U5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V5">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W5" t="s">
         <v>9</v>
@@ -923,7 +923,7 @@
         <v>10</v>
       </c>
       <c r="L6" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="M6" t="s">
         <v>25</v>
@@ -953,11 +953,11 @@
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V6">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W6" t="s">
         <v>17</v>
@@ -998,7 +998,7 @@
         <v>7</v>
       </c>
       <c r="L7" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="M7" t="s">
         <v>25</v>
@@ -1017,18 +1017,18 @@
       </c>
       <c r="R7" s="6">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="S7">
         <v>6</v>
       </c>
       <c r="T7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="U7">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V7">
         <f t="shared" si="4"/>
@@ -1073,7 +1073,7 @@
         <v>10</v>
       </c>
       <c r="L8" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="M8" t="s">
         <v>25</v>
@@ -1092,18 +1092,18 @@
       </c>
       <c r="R8" s="6">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="S8">
         <v>6</v>
       </c>
       <c r="T8">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V8">
         <f t="shared" si="4"/>
@@ -1148,7 +1148,7 @@
         <v>12</v>
       </c>
       <c r="L9" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="M9" t="s">
         <v>25</v>
@@ -1178,11 +1178,11 @@
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V9">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W9" t="s">
         <v>13</v>
@@ -1223,7 +1223,7 @@
         <v>12</v>
       </c>
       <c r="L10" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="M10" t="s">
         <v>25</v>
@@ -1242,18 +1242,18 @@
       </c>
       <c r="R10" s="6">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="S10">
         <v>6</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V10">
         <f t="shared" si="4"/>
@@ -1307,9 +1307,9 @@
         <f t="shared" si="5"/>
         <v>0.4</v>
       </c>
-      <c r="L11" s="5" t="e">
+      <c r="L11" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.8</v>
       </c>
       <c r="M11" s="5" t="e">
         <f t="shared" si="5"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="R11" s="7">
         <f>AVERAGEIF(B11:O11, "&gt;=0")</f>
-        <v>0.6333333333333333</v>
+        <v>0.65</v>
       </c>
       <c r="S11" s="2">
         <f>SUM(S3:S10)</f>
@@ -1341,15 +1341,15 @@
       </c>
       <c r="T11" s="2">
         <f>SUM(T3:T10)</f>
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="U11" s="2">
         <f>SUM(U3:U10)</f>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="V11" s="2">
         <f>SUM(V3:V10)</f>
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1473,7 +1473,7 @@
         <v>7</v>
       </c>
       <c r="L15" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="M15" t="s">
         <v>25</v>
@@ -1503,11 +1503,11 @@
       </c>
       <c r="U15">
         <f t="shared" ref="U15:U20" si="9">COUNTIF(B15:Q15, "A")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V15">
         <f t="shared" ref="V15:V20" si="10">U15-T15</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W15" t="s">
         <v>13</v>
@@ -1548,7 +1548,7 @@
         <v>7</v>
       </c>
       <c r="L16" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="M16" t="s">
         <v>25</v>
@@ -1578,11 +1578,11 @@
       </c>
       <c r="U16">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V16">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W16" t="s">
         <v>15</v>
@@ -1623,7 +1623,7 @@
         <v>10</v>
       </c>
       <c r="L17" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="M17" t="s">
         <v>25</v>
@@ -1642,18 +1642,18 @@
       </c>
       <c r="R17" s="6">
         <f t="shared" si="7"/>
-        <v>0.7142857142857143</v>
+        <v>0.75</v>
       </c>
       <c r="S17">
         <v>10</v>
       </c>
       <c r="T17">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U17">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V17">
         <f t="shared" si="10"/>
@@ -1698,7 +1698,7 @@
         <v>12</v>
       </c>
       <c r="L18" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="M18" t="s">
         <v>25</v>
@@ -1717,18 +1717,18 @@
       </c>
       <c r="R18" s="6">
         <f t="shared" si="7"/>
-        <v>0.5714285714285714</v>
+        <v>0.625</v>
       </c>
       <c r="S18">
         <v>10</v>
       </c>
       <c r="T18">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U18">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V18">
         <f t="shared" si="10"/>
@@ -1773,7 +1773,7 @@
         <v>7</v>
       </c>
       <c r="L19" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="M19" t="s">
         <v>25</v>
@@ -1792,18 +1792,18 @@
       </c>
       <c r="R19" s="6">
         <f t="shared" si="7"/>
-        <v>0.2857142857142857</v>
+        <v>0.375</v>
       </c>
       <c r="S19">
         <v>10</v>
       </c>
       <c r="T19">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U19">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V19">
         <f t="shared" si="10"/>
@@ -1848,7 +1848,7 @@
         <v>12</v>
       </c>
       <c r="L20" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="M20" t="s">
         <v>25</v>
@@ -1878,11 +1878,11 @@
       </c>
       <c r="U20">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V20">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W20" t="s">
         <v>33</v>
@@ -1923,7 +1923,7 @@
         <v>10</v>
       </c>
       <c r="L21" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="M21" t="s">
         <v>25</v>
@@ -1942,18 +1942,18 @@
       </c>
       <c r="R21" s="6">
         <f>COUNTIF(B21:O21, "W")/(COUNTIF(B21:O21, "W")+COUNTIF(B21:O21, "L"))</f>
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="S21">
         <v>6</v>
       </c>
       <c r="T21">
         <f>S21-COUNTIF(B21:Q21, "W")-COUNTIF(B21:Q21, "L")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U21">
         <f>COUNTIF(B21:Q21, "A")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V21">
         <f>U21-T21</f>
@@ -1998,7 +1998,7 @@
         <v>10</v>
       </c>
       <c r="L22" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="M22" t="s">
         <v>25</v>
@@ -2017,18 +2017,18 @@
       </c>
       <c r="R22" s="6">
         <f>COUNTIF(B22:O22, "W")/(COUNTIF(B22:O22, "W")+COUNTIF(B22:O22, "L"))</f>
-        <v>0.42857142857142855</v>
+        <v>0.375</v>
       </c>
       <c r="S22">
         <v>10</v>
       </c>
       <c r="T22">
         <f>S22-COUNTIF(B22:Q22, "W")-COUNTIF(B22:Q22, "L")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U22">
         <f>COUNTIF(B22:Q22, "A")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V22">
         <f>U22-T22</f>
@@ -2082,9 +2082,9 @@
         <f t="shared" ref="K23" si="18">COUNTIF(K15:K22, "W")/(COUNTIF(K15:K22, "W")+COUNTIF(K15:K22, "L"))</f>
         <v>0.4</v>
       </c>
-      <c r="L23" s="5" t="e">
+      <c r="L23" s="5">
         <f t="shared" ref="L23" si="19">COUNTIF(L15:L22, "W")/(COUNTIF(L15:L22, "W")+COUNTIF(L15:L22, "L"))</f>
-        <v>#DIV/0!</v>
+        <v>0.8</v>
       </c>
       <c r="M23" s="5" t="e">
         <f t="shared" ref="M23" si="20">COUNTIF(M15:M22, "W")/(COUNTIF(M15:M22, "W")+COUNTIF(M15:M22, "L"))</f>
@@ -2108,7 +2108,7 @@
       </c>
       <c r="R23" s="7">
         <f>AVERAGEIF(B23:O23, "&gt;=0")</f>
-        <v>0.54</v>
+        <v>0.5636363636363636</v>
       </c>
       <c r="S23" s="2">
         <f>SUM(S15:S22)</f>
@@ -2116,15 +2116,15 @@
       </c>
       <c r="T23" s="2">
         <f>SUM(T15:T22)</f>
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="U23" s="2">
         <f>SUM(U15:U22)</f>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="V23" s="2">
         <f>SUM(V15:V22)</f>
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall 22 week 12 day-after inputs
</commit_message>
<xml_diff>
--- a/data/Fall2022Schedule.xlsx
+++ b/data/Fall2022Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B5F007-F3A6-4B37-9E76-DEB32C2DB08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8BC030-A9C9-4468-82F9-2872AE0B2015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18435" yWindow="2025" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
   </bookViews>
@@ -552,9 +552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA30A97-9145-4EDA-8DB9-44B6A1233BAB}">
   <dimension ref="A2:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +701,7 @@
         <v>12</v>
       </c>
       <c r="M3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="N3" t="s">
         <v>25</v>
@@ -717,18 +717,18 @@
       </c>
       <c r="R3" s="6">
         <f t="shared" ref="R3:R10" si="1">COUNTIF(B3:O3, "W")/(COUNTIF(B3:O3, "W")+COUNTIF(B3:O3, "L"))</f>
-        <v>0.66666666666666663</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="S3">
         <v>6</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T10" si="2">S3-COUNTIF(B3:Q3, "W")-COUNTIF(B3:Q3, "L")</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U10" si="3">COUNTIF(B3:Q3, "A")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V10" si="4">U3-T3</f>
@@ -776,7 +776,7 @@
         <v>12</v>
       </c>
       <c r="M4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="N4" t="s">
         <v>25</v>
@@ -792,18 +792,18 @@
       </c>
       <c r="R4" s="6">
         <f t="shared" si="1"/>
-        <v>0.625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S4">
         <v>6</v>
       </c>
       <c r="T4">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="U4">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V4">
         <f t="shared" si="4"/>
@@ -851,7 +851,7 @@
         <v>10</v>
       </c>
       <c r="M5" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="N5" t="s">
         <v>25</v>
@@ -878,11 +878,11 @@
       </c>
       <c r="U5">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V5">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W5" t="s">
         <v>9</v>
@@ -926,7 +926,7 @@
         <v>8</v>
       </c>
       <c r="M6" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="N6" t="s">
         <v>25</v>
@@ -942,18 +942,18 @@
       </c>
       <c r="R6" s="6">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S6">
         <v>6</v>
       </c>
       <c r="T6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V6">
         <f t="shared" si="4"/>
@@ -1001,7 +1001,7 @@
         <v>7</v>
       </c>
       <c r="M7" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="N7" t="s">
         <v>25</v>
@@ -1028,11 +1028,11 @@
       </c>
       <c r="U7">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V7">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W7" t="s">
         <v>20</v>
@@ -1076,7 +1076,7 @@
         <v>12</v>
       </c>
       <c r="M8" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="N8" t="s">
         <v>25</v>
@@ -1092,18 +1092,18 @@
       </c>
       <c r="R8" s="6">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="S8">
         <v>6</v>
       </c>
       <c r="T8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V8">
         <f t="shared" si="4"/>
@@ -1151,7 +1151,7 @@
         <v>8</v>
       </c>
       <c r="M9" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="N9" t="s">
         <v>25</v>
@@ -1178,11 +1178,11 @@
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V9">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W9" t="s">
         <v>13</v>
@@ -1226,7 +1226,7 @@
         <v>12</v>
       </c>
       <c r="M10" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="N10" t="s">
         <v>25</v>
@@ -1242,18 +1242,18 @@
       </c>
       <c r="R10" s="6">
         <f t="shared" si="1"/>
-        <v>0.5714285714285714</v>
+        <v>0.625</v>
       </c>
       <c r="S10">
         <v>6</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V10">
         <f t="shared" si="4"/>
@@ -1311,9 +1311,9 @@
         <f t="shared" si="5"/>
         <v>0.8</v>
       </c>
-      <c r="M11" s="5" t="e">
+      <c r="M11" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.6</v>
       </c>
       <c r="N11" s="5" t="e">
         <f t="shared" si="5"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="R11" s="7">
         <f>AVERAGEIF(B11:O11, "&gt;=0")</f>
-        <v>0.65</v>
+        <v>0.64545454545454539</v>
       </c>
       <c r="S11" s="2">
         <f>SUM(S3:S10)</f>
@@ -1341,15 +1341,15 @@
       </c>
       <c r="T11" s="2">
         <f>SUM(T3:T10)</f>
-        <v>-1</v>
+        <v>-6</v>
       </c>
       <c r="U11" s="2">
         <f>SUM(U3:U10)</f>
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="V11" s="2">
         <f>SUM(V3:V10)</f>
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1476,7 +1476,7 @@
         <v>8</v>
       </c>
       <c r="M15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="N15" t="s">
         <v>25</v>
@@ -1492,18 +1492,18 @@
       </c>
       <c r="R15" s="6">
         <f t="shared" ref="R15:R20" si="7">COUNTIF(B15:O15, "W")/(COUNTIF(B15:O15, "W")+COUNTIF(B15:O15, "L"))</f>
-        <v>0.42857142857142855</v>
+        <v>0.5</v>
       </c>
       <c r="S15">
         <v>10</v>
       </c>
       <c r="T15">
         <f t="shared" ref="T15:T20" si="8">S15-COUNTIF(B15:Q15, "W")-COUNTIF(B15:Q15, "L")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U15">
         <f t="shared" ref="U15:U20" si="9">COUNTIF(B15:Q15, "A")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V15">
         <f t="shared" ref="V15:V20" si="10">U15-T15</f>
@@ -1551,7 +1551,7 @@
         <v>10</v>
       </c>
       <c r="M16" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="N16" t="s">
         <v>25</v>
@@ -1567,18 +1567,18 @@
       </c>
       <c r="R16" s="6">
         <f t="shared" si="7"/>
-        <v>0.5714285714285714</v>
+        <v>0.625</v>
       </c>
       <c r="S16">
         <v>10</v>
       </c>
       <c r="T16">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U16">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V16">
         <f t="shared" si="10"/>
@@ -1626,7 +1626,7 @@
         <v>12</v>
       </c>
       <c r="M17" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="N17" t="s">
         <v>25</v>
@@ -1653,11 +1653,11 @@
       </c>
       <c r="U17">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V17">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W17" t="s">
         <v>28</v>
@@ -1701,7 +1701,7 @@
         <v>12</v>
       </c>
       <c r="M18" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="N18" t="s">
         <v>25</v>
@@ -1728,11 +1728,11 @@
       </c>
       <c r="U18">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V18">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W18" t="s">
         <v>20</v>
@@ -1776,7 +1776,7 @@
         <v>12</v>
       </c>
       <c r="M19" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="N19" t="s">
         <v>25</v>
@@ -1803,11 +1803,11 @@
       </c>
       <c r="U19">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V19">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W19" t="s">
         <v>22</v>
@@ -1851,7 +1851,7 @@
         <v>10</v>
       </c>
       <c r="M20" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="N20" t="s">
         <v>25</v>
@@ -1867,18 +1867,18 @@
       </c>
       <c r="R20" s="6">
         <f t="shared" si="7"/>
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="S20">
         <v>6</v>
       </c>
       <c r="T20">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U20">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V20">
         <f t="shared" si="10"/>
@@ -1926,7 +1926,7 @@
         <v>12</v>
       </c>
       <c r="M21" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="N21" t="s">
         <v>25</v>
@@ -1942,18 +1942,18 @@
       </c>
       <c r="R21" s="6">
         <f>COUNTIF(B21:O21, "W")/(COUNTIF(B21:O21, "W")+COUNTIF(B21:O21, "L"))</f>
-        <v>0.8</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="S21">
         <v>6</v>
       </c>
       <c r="T21">
         <f>S21-COUNTIF(B21:Q21, "W")-COUNTIF(B21:Q21, "L")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U21">
         <f>COUNTIF(B21:Q21, "A")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V21">
         <f>U21-T21</f>
@@ -2001,7 +2001,7 @@
         <v>7</v>
       </c>
       <c r="M22" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="N22" t="s">
         <v>25</v>
@@ -2017,18 +2017,18 @@
       </c>
       <c r="R22" s="6">
         <f>COUNTIF(B22:O22, "W")/(COUNTIF(B22:O22, "W")+COUNTIF(B22:O22, "L"))</f>
-        <v>0.375</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="S22">
         <v>10</v>
       </c>
       <c r="T22">
         <f>S22-COUNTIF(B22:Q22, "W")-COUNTIF(B22:Q22, "L")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U22">
         <f>COUNTIF(B22:Q22, "A")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V22">
         <f>U22-T22</f>
@@ -2086,9 +2086,9 @@
         <f t="shared" ref="L23" si="19">COUNTIF(L15:L22, "W")/(COUNTIF(L15:L22, "W")+COUNTIF(L15:L22, "L"))</f>
         <v>0.8</v>
       </c>
-      <c r="M23" s="5" t="e">
+      <c r="M23" s="5">
         <f t="shared" ref="M23" si="20">COUNTIF(M15:M22, "W")/(COUNTIF(M15:M22, "W")+COUNTIF(M15:M22, "L"))</f>
-        <v>#DIV/0!</v>
+        <v>0.8</v>
       </c>
       <c r="N23" s="5" t="e">
         <f t="shared" ref="N23" si="21">COUNTIF(N15:N22, "W")/(COUNTIF(N15:N22, "W")+COUNTIF(N15:N22, "L"))</f>
@@ -2108,7 +2108,7 @@
       </c>
       <c r="R23" s="7">
         <f>AVERAGEIF(B23:O23, "&gt;=0")</f>
-        <v>0.5636363636363636</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="S23" s="2">
         <f>SUM(S15:S22)</f>
@@ -2116,15 +2116,15 @@
       </c>
       <c r="T23" s="2">
         <f>SUM(T15:T22)</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="U23" s="2">
         <f>SUM(U15:U22)</f>
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="V23" s="2">
         <f>SUM(V15:V22)</f>
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall 22 week 12 complete
</commit_message>
<xml_diff>
--- a/data/Fall2022Schedule.xlsx
+++ b/data/Fall2022Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8BC030-A9C9-4468-82F9-2872AE0B2015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43034BFA-876E-4D1A-8D97-3AD3826707E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18435" yWindow="2025" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
   </bookViews>
@@ -552,9 +552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA30A97-9145-4EDA-8DB9-44B6A1233BAB}">
   <dimension ref="A2:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V23" sqref="V23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +689,7 @@
         <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J3" t="s">
         <v>10</v>
@@ -764,7 +764,7 @@
         <v>7</v>
       </c>
       <c r="I4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J4" t="s">
         <v>12</v>
@@ -839,7 +839,7 @@
         <v>7</v>
       </c>
       <c r="I5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J5" t="s">
         <v>8</v>
@@ -914,7 +914,7 @@
         <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J6" t="s">
         <v>12</v>
@@ -989,7 +989,7 @@
         <v>12</v>
       </c>
       <c r="I7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J7" t="s">
         <v>10</v>
@@ -1064,7 +1064,7 @@
         <v>12</v>
       </c>
       <c r="I8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J8" t="s">
         <v>7</v>
@@ -1139,7 +1139,7 @@
         <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J9" t="s">
         <v>7</v>
@@ -1214,7 +1214,7 @@
         <v>7</v>
       </c>
       <c r="I10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J10" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
fall 22 week 13 day-after inputs
</commit_message>
<xml_diff>
--- a/data/Fall2022Schedule.xlsx
+++ b/data/Fall2022Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43034BFA-876E-4D1A-8D97-3AD3826707E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197F3180-BBA9-44B3-BFB6-636A5FE50EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18435" yWindow="2025" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
   </bookViews>
@@ -554,7 +554,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K12" sqref="K12"/>
+      <selection pane="topRight" activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +704,7 @@
         <v>7</v>
       </c>
       <c r="N3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="O3" t="s">
         <v>25</v>
@@ -717,18 +717,18 @@
       </c>
       <c r="R3" s="6">
         <f t="shared" ref="R3:R10" si="1">COUNTIF(B3:O3, "W")/(COUNTIF(B3:O3, "W")+COUNTIF(B3:O3, "L"))</f>
-        <v>0.5714285714285714</v>
+        <v>0.625</v>
       </c>
       <c r="S3">
         <v>6</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T10" si="2">S3-COUNTIF(B3:Q3, "W")-COUNTIF(B3:Q3, "L")</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U10" si="3">COUNTIF(B3:Q3, "A")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V10" si="4">U3-T3</f>
@@ -779,7 +779,7 @@
         <v>12</v>
       </c>
       <c r="N4" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="O4" t="s">
         <v>25</v>
@@ -792,18 +792,18 @@
       </c>
       <c r="R4" s="6">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>0.6</v>
       </c>
       <c r="S4">
         <v>6</v>
       </c>
       <c r="T4">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="U4">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V4">
         <f t="shared" si="4"/>
@@ -854,7 +854,7 @@
         <v>8</v>
       </c>
       <c r="N5" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="O5" t="s">
         <v>25</v>
@@ -867,18 +867,18 @@
       </c>
       <c r="R5" s="6">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="S5">
         <v>6</v>
       </c>
       <c r="T5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="U5">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V5">
         <f t="shared" si="4"/>
@@ -929,7 +929,7 @@
         <v>7</v>
       </c>
       <c r="N6" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="O6" t="s">
         <v>25</v>
@@ -953,11 +953,11 @@
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V6">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W6" t="s">
         <v>17</v>
@@ -1004,7 +1004,7 @@
         <v>8</v>
       </c>
       <c r="N7" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="O7" t="s">
         <v>25</v>
@@ -1028,11 +1028,11 @@
       </c>
       <c r="U7">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V7">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W7" t="s">
         <v>20</v>
@@ -1079,7 +1079,7 @@
         <v>12</v>
       </c>
       <c r="N8" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="O8" t="s">
         <v>25</v>
@@ -1103,11 +1103,11 @@
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V8">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W8" t="s">
         <v>15</v>
@@ -1154,7 +1154,7 @@
         <v>10</v>
       </c>
       <c r="N9" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="O9" t="s">
         <v>25</v>
@@ -1178,11 +1178,11 @@
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V9">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W9" t="s">
         <v>13</v>
@@ -1229,7 +1229,7 @@
         <v>12</v>
       </c>
       <c r="N10" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="O10" t="s">
         <v>25</v>
@@ -1242,18 +1242,18 @@
       </c>
       <c r="R10" s="6">
         <f t="shared" si="1"/>
-        <v>0.625</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="S10">
         <v>6</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V10">
         <f t="shared" si="4"/>
@@ -1315,9 +1315,9 @@
         <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
-      <c r="N11" s="5" t="e">
+      <c r="N11" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.25</v>
       </c>
       <c r="O11" s="5" t="e">
         <f t="shared" si="5"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="R11" s="7">
         <f>AVERAGEIF(B11:O11, "&gt;=0")</f>
-        <v>0.64545454545454539</v>
+        <v>0.61249999999999993</v>
       </c>
       <c r="S11" s="2">
         <f>SUM(S3:S10)</f>
@@ -1341,15 +1341,15 @@
       </c>
       <c r="T11" s="2">
         <f>SUM(T3:T10)</f>
-        <v>-6</v>
+        <v>-10</v>
       </c>
       <c r="U11" s="2">
         <f>SUM(U3:U10)</f>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="V11" s="2">
         <f>SUM(V3:V10)</f>
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1479,7 +1479,7 @@
         <v>12</v>
       </c>
       <c r="N15" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="O15" t="s">
         <v>25</v>
@@ -1503,11 +1503,11 @@
       </c>
       <c r="U15">
         <f t="shared" ref="U15:U20" si="9">COUNTIF(B15:Q15, "A")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V15">
         <f t="shared" ref="V15:V20" si="10">U15-T15</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W15" t="s">
         <v>13</v>
@@ -1551,10 +1551,10 @@
         <v>10</v>
       </c>
       <c r="M16" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="N16" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="O16" t="s">
         <v>25</v>
@@ -1567,18 +1567,18 @@
       </c>
       <c r="R16" s="6">
         <f t="shared" si="7"/>
-        <v>0.625</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="S16">
         <v>10</v>
       </c>
       <c r="T16">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U16">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V16">
         <f t="shared" si="10"/>
@@ -1629,7 +1629,7 @@
         <v>10</v>
       </c>
       <c r="N17" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="O17" t="s">
         <v>25</v>
@@ -1642,18 +1642,18 @@
       </c>
       <c r="R17" s="6">
         <f t="shared" si="7"/>
-        <v>0.75</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="S17">
         <v>10</v>
       </c>
       <c r="T17">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U17">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V17">
         <f t="shared" si="10"/>
@@ -1704,7 +1704,7 @@
         <v>8</v>
       </c>
       <c r="N18" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="O18" t="s">
         <v>25</v>
@@ -1717,18 +1717,18 @@
       </c>
       <c r="R18" s="6">
         <f t="shared" si="7"/>
-        <v>0.625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S18">
         <v>10</v>
       </c>
       <c r="T18">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U18">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V18">
         <f t="shared" si="10"/>
@@ -1779,7 +1779,7 @@
         <v>10</v>
       </c>
       <c r="N19" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="O19" t="s">
         <v>25</v>
@@ -1792,18 +1792,18 @@
       </c>
       <c r="R19" s="6">
         <f t="shared" si="7"/>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="S19">
         <v>10</v>
       </c>
       <c r="T19">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U19">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V19">
         <f t="shared" si="10"/>
@@ -1854,7 +1854,7 @@
         <v>7</v>
       </c>
       <c r="N20" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="O20" t="s">
         <v>25</v>
@@ -1878,11 +1878,11 @@
       </c>
       <c r="U20">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V20">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W20" t="s">
         <v>33</v>
@@ -1929,7 +1929,7 @@
         <v>12</v>
       </c>
       <c r="N21" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="O21" t="s">
         <v>25</v>
@@ -1953,11 +1953,11 @@
       </c>
       <c r="U21">
         <f>COUNTIF(B21:Q21, "A")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V21">
         <f>U21-T21</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W21" t="s">
         <v>32</v>
@@ -2004,7 +2004,7 @@
         <v>12</v>
       </c>
       <c r="N22" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="O22" t="s">
         <v>25</v>
@@ -2017,18 +2017,18 @@
       </c>
       <c r="R22" s="6">
         <f>COUNTIF(B22:O22, "W")/(COUNTIF(B22:O22, "W")+COUNTIF(B22:O22, "L"))</f>
-        <v>0.44444444444444442</v>
+        <v>0.5</v>
       </c>
       <c r="S22">
         <v>10</v>
       </c>
       <c r="T22">
         <f>S22-COUNTIF(B22:Q22, "W")-COUNTIF(B22:Q22, "L")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U22">
         <f>COUNTIF(B22:Q22, "A")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V22">
         <f>U22-T22</f>
@@ -2088,11 +2088,11 @@
       </c>
       <c r="M23" s="5">
         <f t="shared" ref="M23" si="20">COUNTIF(M15:M22, "W")/(COUNTIF(M15:M22, "W")+COUNTIF(M15:M22, "L"))</f>
+        <v>0.6</v>
+      </c>
+      <c r="N23" s="5">
+        <f t="shared" ref="N23" si="21">COUNTIF(N15:N22, "W")/(COUNTIF(N15:N22, "W")+COUNTIF(N15:N22, "L"))</f>
         <v>0.8</v>
-      </c>
-      <c r="N23" s="5" t="e">
-        <f t="shared" ref="N23" si="21">COUNTIF(N15:N22, "W")/(COUNTIF(N15:N22, "W")+COUNTIF(N15:N22, "L"))</f>
-        <v>#DIV/0!</v>
       </c>
       <c r="O23" s="5" t="e">
         <f t="shared" ref="O23" si="22">COUNTIF(O15:O22, "W")/(COUNTIF(O15:O22, "W")+COUNTIF(O15:O22, "L"))</f>
@@ -2108,7 +2108,7 @@
       </c>
       <c r="R23" s="7">
         <f>AVERAGEIF(B23:O23, "&gt;=0")</f>
-        <v>0.58333333333333337</v>
+        <v>0.58461538461538454</v>
       </c>
       <c r="S23" s="2">
         <f>SUM(S15:S22)</f>
@@ -2116,15 +2116,15 @@
       </c>
       <c r="T23" s="2">
         <f>SUM(T15:T22)</f>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="U23" s="2">
         <f>SUM(U15:U22)</f>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="V23" s="2">
         <f>SUM(V15:V22)</f>
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall 22 week 14 day-after
</commit_message>
<xml_diff>
--- a/data/Fall2022Schedule.xlsx
+++ b/data/Fall2022Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815938FC-FE0A-41BF-B2A2-3A3507E1CA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7793E3FF-6C12-4FD4-86A0-6FE4BE6F0885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18435" yWindow="2025" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
   </bookViews>
@@ -552,9 +552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA30A97-9145-4EDA-8DB9-44B6A1233BAB}">
   <dimension ref="A2:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U3" sqref="U3"/>
+      <selection pane="topRight" activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +707,7 @@
         <v>12</v>
       </c>
       <c r="O3" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
@@ -728,11 +728,11 @@
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U10" si="2">COUNTIF(B3:Q3, "A")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V10" si="3">U3-T3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W3" t="s">
         <v>28</v>
@@ -782,7 +782,7 @@
         <v>7</v>
       </c>
       <c r="O4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="P4" t="s">
         <v>25</v>
@@ -803,11 +803,11 @@
       </c>
       <c r="U4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V4">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W4" t="s">
         <v>24</v>
@@ -857,7 +857,7 @@
         <v>7</v>
       </c>
       <c r="O5" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="P5" t="s">
         <v>25</v>
@@ -878,11 +878,11 @@
       </c>
       <c r="U5">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W5" t="s">
         <v>9</v>
@@ -932,7 +932,7 @@
         <v>8</v>
       </c>
       <c r="O6" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="P6" t="s">
         <v>25</v>
@@ -942,7 +942,7 @@
       </c>
       <c r="R6" s="6">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="S6">
         <v>6</v>
@@ -953,11 +953,11 @@
       </c>
       <c r="U6">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V6">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W6" t="s">
         <v>17</v>
@@ -1007,7 +1007,7 @@
         <v>10</v>
       </c>
       <c r="O7" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="P7" t="s">
         <v>25</v>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="R7" s="6">
         <f t="shared" si="1"/>
-        <v>0.5714285714285714</v>
+        <v>0.625</v>
       </c>
       <c r="S7">
         <v>6</v>
@@ -1028,11 +1028,11 @@
       </c>
       <c r="U7">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V7">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W7" t="s">
         <v>20</v>
@@ -1082,7 +1082,7 @@
         <v>10</v>
       </c>
       <c r="O8" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="P8" t="s">
         <v>25</v>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="R8" s="6">
         <f t="shared" si="1"/>
-        <v>0.8571428571428571</v>
+        <v>0.875</v>
       </c>
       <c r="S8">
         <v>6</v>
@@ -1103,11 +1103,11 @@
       </c>
       <c r="U8">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V8">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W8" t="s">
         <v>15</v>
@@ -1157,7 +1157,7 @@
         <v>8</v>
       </c>
       <c r="O9" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="P9" t="s">
         <v>25</v>
@@ -1167,18 +1167,18 @@
       </c>
       <c r="R9" s="6">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="S9">
         <v>6</v>
       </c>
       <c r="T9">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U9">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V9">
         <f t="shared" si="3"/>
@@ -1232,7 +1232,7 @@
         <v>7</v>
       </c>
       <c r="O10" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="P10" t="s">
         <v>25</v>
@@ -1242,7 +1242,7 @@
       </c>
       <c r="R10" s="6">
         <f t="shared" si="1"/>
-        <v>0.55555555555555558</v>
+        <v>0.5</v>
       </c>
       <c r="S10">
         <v>6</v>
@@ -1253,11 +1253,11 @@
       </c>
       <c r="U10">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V10">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W10" t="s">
         <v>22</v>
@@ -1319,9 +1319,9 @@
         <f t="shared" si="5"/>
         <v>0.25</v>
       </c>
-      <c r="O11" s="5" t="e">
+      <c r="O11" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.4</v>
       </c>
       <c r="P11" s="5" t="e">
         <f t="shared" si="5"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="R11" s="7">
         <f>AVERAGEIF(B11:O11, "&gt;=0")</f>
-        <v>0.61249999999999993</v>
+        <v>0.59615384615384615</v>
       </c>
       <c r="S11" s="2">
         <f>SUM(S3:S10)</f>
@@ -1341,15 +1341,15 @@
       </c>
       <c r="T11" s="2">
         <f>SUM(T3:T10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U11" s="2">
         <f>SUM(U3:U10)</f>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="V11" s="2">
         <f>SUM(V3:V10)</f>
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1482,7 +1482,7 @@
         <v>8</v>
       </c>
       <c r="O15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="P15" t="s">
         <v>25</v>
@@ -1492,18 +1492,18 @@
       </c>
       <c r="R15" s="6">
         <f t="shared" ref="R15:R20" si="7">COUNTIF(B15:O15, "W")/(COUNTIF(B15:O15, "W")+COUNTIF(B15:O15, "L"))</f>
-        <v>0.5</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="S15">
         <v>10</v>
       </c>
       <c r="T15">
         <f>MAX(S15-COUNTIF(B15:Q15, "W")-COUNTIF(B15:Q15, "L"), 0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U15">
         <f t="shared" ref="U15:U20" si="8">COUNTIF(B15:Q15, "A")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V15">
         <f t="shared" ref="V15:V20" si="9">U15-T15</f>
@@ -1557,7 +1557,7 @@
         <v>12</v>
       </c>
       <c r="O16" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="P16" t="s">
         <v>25</v>
@@ -1567,18 +1567,18 @@
       </c>
       <c r="R16" s="6">
         <f t="shared" si="7"/>
-        <v>0.55555555555555558</v>
+        <v>0.6</v>
       </c>
       <c r="S16">
         <v>10</v>
       </c>
       <c r="T16">
         <f t="shared" ref="T16:T22" si="10">MAX(S16-COUNTIF(B16:Q16, "W")-COUNTIF(B16:Q16, "L"), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U16">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V16">
         <f t="shared" si="9"/>
@@ -1632,7 +1632,7 @@
         <v>12</v>
       </c>
       <c r="O17" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="P17" t="s">
         <v>25</v>
@@ -1653,11 +1653,11 @@
       </c>
       <c r="U17">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V17">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W17" t="s">
         <v>28</v>
@@ -1707,7 +1707,7 @@
         <v>12</v>
       </c>
       <c r="O18" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="P18" t="s">
         <v>25</v>
@@ -1717,18 +1717,18 @@
       </c>
       <c r="R18" s="6">
         <f t="shared" si="7"/>
-        <v>0.66666666666666663</v>
+        <v>0.6</v>
       </c>
       <c r="S18">
         <v>10</v>
       </c>
       <c r="T18">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U18">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V18">
         <f t="shared" si="9"/>
@@ -1782,7 +1782,7 @@
         <v>7</v>
       </c>
       <c r="O19" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="P19" t="s">
         <v>25</v>
@@ -1803,11 +1803,11 @@
       </c>
       <c r="U19">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V19">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W19" t="s">
         <v>22</v>
@@ -1857,7 +1857,7 @@
         <v>10</v>
       </c>
       <c r="O20" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="P20" t="s">
         <v>25</v>
@@ -1867,18 +1867,18 @@
       </c>
       <c r="R20" s="6">
         <f t="shared" si="7"/>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="S20">
         <v>6</v>
       </c>
       <c r="T20">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U20">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V20">
         <f t="shared" si="9"/>
@@ -1932,7 +1932,7 @@
         <v>8</v>
       </c>
       <c r="O21" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="P21" t="s">
         <v>25</v>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="R21" s="6">
         <f>COUNTIF(B21:O21, "W")/(COUNTIF(B21:O21, "W")+COUNTIF(B21:O21, "L"))</f>
-        <v>0.83333333333333337</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="S21">
         <v>6</v>
@@ -1953,11 +1953,11 @@
       </c>
       <c r="U21">
         <f>COUNTIF(B21:Q21, "A")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V21">
         <f>U21-T21</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W21" t="s">
         <v>32</v>
@@ -2007,7 +2007,7 @@
         <v>12</v>
       </c>
       <c r="O22" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="P22" t="s">
         <v>25</v>
@@ -2028,11 +2028,11 @@
       </c>
       <c r="U22">
         <f>COUNTIF(B22:Q22, "A")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V22">
         <f>U22-T22</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W22" t="s">
         <v>35</v>
@@ -2094,9 +2094,9 @@
         <f t="shared" ref="N23" si="21">COUNTIF(N15:N22, "W")/(COUNTIF(N15:N22, "W")+COUNTIF(N15:N22, "L"))</f>
         <v>0.8</v>
       </c>
-      <c r="O23" s="5" t="e">
+      <c r="O23" s="5">
         <f t="shared" ref="O23" si="22">COUNTIF(O15:O22, "W")/(COUNTIF(O15:O22, "W")+COUNTIF(O15:O22, "L"))</f>
-        <v>#DIV/0!</v>
+        <v>0.6</v>
       </c>
       <c r="P23" s="5" t="e">
         <f t="shared" ref="P23" si="23">COUNTIF(P15:P22, "W")/(COUNTIF(P15:P22, "W")+COUNTIF(P15:P22, "L"))</f>
@@ -2108,7 +2108,7 @@
       </c>
       <c r="R23" s="7">
         <f>AVERAGEIF(B23:O23, "&gt;=0")</f>
-        <v>0.58461538461538454</v>
+        <v>0.58571428571428563</v>
       </c>
       <c r="S23" s="2">
         <f>SUM(S15:S22)</f>
@@ -2116,15 +2116,15 @@
       </c>
       <c r="T23" s="2">
         <f>SUM(T15:T22)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="U23" s="2">
         <f>SUM(U15:U22)</f>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="V23" s="2">
         <f>SUM(V15:V22)</f>
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall 22 week 15 day-after inputs
</commit_message>
<xml_diff>
--- a/data/Fall2022Schedule.xlsx
+++ b/data/Fall2022Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7793E3FF-6C12-4FD4-86A0-6FE4BE6F0885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB34328E-AE33-49E2-AD31-5C411726E357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18435" yWindow="2025" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
   </bookViews>
@@ -552,9 +552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA30A97-9145-4EDA-8DB9-44B6A1233BAB}">
   <dimension ref="A2:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P26" sqref="P26"/>
+      <selection pane="topRight" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +710,7 @@
         <v>8</v>
       </c>
       <c r="P3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="Q3" t="s">
         <v>25</v>
@@ -728,11 +728,11 @@
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U10" si="2">COUNTIF(B3:Q3, "A")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V10" si="3">U3-T3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W3" t="s">
         <v>28</v>
@@ -785,7 +785,7 @@
         <v>10</v>
       </c>
       <c r="P4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="Q4" t="s">
         <v>25</v>
@@ -803,11 +803,11 @@
       </c>
       <c r="U4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V4">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W4" t="s">
         <v>24</v>
@@ -860,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="P5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="Q5" t="s">
         <v>25</v>
@@ -878,11 +878,11 @@
       </c>
       <c r="U5">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W5" t="s">
         <v>9</v>
@@ -935,7 +935,7 @@
         <v>7</v>
       </c>
       <c r="P6" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="Q6" t="s">
         <v>25</v>
@@ -953,11 +953,11 @@
       </c>
       <c r="U6">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V6">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W6" t="s">
         <v>17</v>
@@ -1010,7 +1010,7 @@
         <v>12</v>
       </c>
       <c r="P7" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="Q7" t="s">
         <v>25</v>
@@ -1028,11 +1028,11 @@
       </c>
       <c r="U7">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V7">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W7" t="s">
         <v>20</v>
@@ -1085,7 +1085,7 @@
         <v>12</v>
       </c>
       <c r="P8" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="Q8" t="s">
         <v>25</v>
@@ -1103,11 +1103,11 @@
       </c>
       <c r="U8">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W8" t="s">
         <v>15</v>
@@ -1160,7 +1160,7 @@
         <v>7</v>
       </c>
       <c r="P9" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="Q9" t="s">
         <v>25</v>
@@ -1174,11 +1174,11 @@
       </c>
       <c r="T9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U9">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V9">
         <f t="shared" si="3"/>
@@ -1235,7 +1235,7 @@
         <v>7</v>
       </c>
       <c r="P10" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="Q10" t="s">
         <v>25</v>
@@ -1253,11 +1253,11 @@
       </c>
       <c r="U10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V10">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W10" t="s">
         <v>22</v>
@@ -1323,9 +1323,9 @@
         <f t="shared" si="5"/>
         <v>0.4</v>
       </c>
-      <c r="P11" s="5" t="e">
+      <c r="P11" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="5" t="e">
         <f t="shared" si="5"/>
@@ -1341,15 +1341,15 @@
       </c>
       <c r="T11" s="2">
         <f>SUM(T3:T10)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" s="2">
         <f>SUM(U3:U10)</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="V11" s="2">
         <f>SUM(V3:V10)</f>
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1485,7 +1485,7 @@
         <v>12</v>
       </c>
       <c r="P15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="Q15" t="s">
         <v>25</v>
@@ -1499,11 +1499,11 @@
       </c>
       <c r="T15">
         <f>MAX(S15-COUNTIF(B15:Q15, "W")-COUNTIF(B15:Q15, "L"), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15">
         <f t="shared" ref="U15:U20" si="8">COUNTIF(B15:Q15, "A")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V15">
         <f t="shared" ref="V15:V20" si="9">U15-T15</f>
@@ -1560,7 +1560,7 @@
         <v>12</v>
       </c>
       <c r="P16" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="Q16" t="s">
         <v>25</v>
@@ -1578,11 +1578,11 @@
       </c>
       <c r="U16">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V16">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W16" t="s">
         <v>15</v>
@@ -1635,7 +1635,7 @@
         <v>8</v>
       </c>
       <c r="P17" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="Q17" t="s">
         <v>25</v>
@@ -1649,11 +1649,11 @@
       </c>
       <c r="T17">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V17">
         <f t="shared" si="9"/>
@@ -1710,7 +1710,7 @@
         <v>7</v>
       </c>
       <c r="P18" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="Q18" t="s">
         <v>25</v>
@@ -1728,11 +1728,11 @@
       </c>
       <c r="U18">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V18">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W18" t="s">
         <v>20</v>
@@ -1785,7 +1785,7 @@
         <v>10</v>
       </c>
       <c r="P19" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="Q19" t="s">
         <v>25</v>
@@ -1799,11 +1799,11 @@
       </c>
       <c r="T19">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U19">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V19">
         <f t="shared" si="9"/>
@@ -1860,7 +1860,7 @@
         <v>7</v>
       </c>
       <c r="P20" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="Q20" t="s">
         <v>25</v>
@@ -1878,11 +1878,11 @@
       </c>
       <c r="U20">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V20">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W20" t="s">
         <v>33</v>
@@ -1935,7 +1935,7 @@
         <v>12</v>
       </c>
       <c r="P21" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="Q21" t="s">
         <v>25</v>
@@ -1953,11 +1953,11 @@
       </c>
       <c r="U21">
         <f>COUNTIF(B21:Q21, "A")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V21">
         <f>U21-T21</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W21" t="s">
         <v>32</v>
@@ -2010,7 +2010,7 @@
         <v>10</v>
       </c>
       <c r="P22" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="Q22" t="s">
         <v>25</v>
@@ -2028,11 +2028,11 @@
       </c>
       <c r="U22">
         <f>COUNTIF(B22:Q22, "A")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V22">
         <f>U22-T22</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W22" t="s">
         <v>35</v>
@@ -2098,9 +2098,9 @@
         <f t="shared" ref="O23" si="22">COUNTIF(O15:O22, "W")/(COUNTIF(O15:O22, "W")+COUNTIF(O15:O22, "L"))</f>
         <v>0.6</v>
       </c>
-      <c r="P23" s="5" t="e">
+      <c r="P23" s="5">
         <f t="shared" ref="P23" si="23">COUNTIF(P15:P22, "W")/(COUNTIF(P15:P22, "W")+COUNTIF(P15:P22, "L"))</f>
-        <v>#DIV/0!</v>
+        <v>0.5</v>
       </c>
       <c r="Q23" s="5" t="e">
         <f t="shared" ref="Q23" si="24">COUNTIF(Q15:Q22, "W")/(COUNTIF(Q15:Q22, "W")+COUNTIF(Q15:Q22, "L"))</f>
@@ -2116,15 +2116,15 @@
       </c>
       <c r="T23" s="2">
         <f>SUM(T15:T22)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U23" s="2">
         <f>SUM(U15:U22)</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="V23" s="2">
         <f>SUM(V15:V22)</f>
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall 22 week 16 day after inputs
</commit_message>
<xml_diff>
--- a/data/Fall2022Schedule.xlsx
+++ b/data/Fall2022Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB34328E-AE33-49E2-AD31-5C411726E357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABDC27D-65F0-45F3-BA68-764EE9DE3C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18435" yWindow="2025" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="35">
   <si>
     <t>Record</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>678-508-0979</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
   <si>
     <t>Daniel Burcham</t>
@@ -554,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q13" sqref="Q13"/>
+      <selection pane="topRight" activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +576,7 @@
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1">
         <v>44803</v>
@@ -665,7 +662,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -713,11 +710,11 @@
         <v>10</v>
       </c>
       <c r="Q3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="R3" s="6">
-        <f t="shared" ref="R3:R10" si="1">COUNTIF(B3:O3, "W")/(COUNTIF(B3:O3, "W")+COUNTIF(B3:O3, "L"))</f>
-        <v>0.625</v>
+        <f>COUNTIF(B3:Q3, "W")/(COUNTIF(B3:Q3, "W")+COUNTIF(B3:Q3, "L"))</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S3">
         <v>6</v>
@@ -727,15 +724,15 @@
         <v>0</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U10" si="2">COUNTIF(B3:Q3, "A")</f>
-        <v>1</v>
+        <f t="shared" ref="U3:U10" si="1">COUNTIF(B3:Q3, "A")</f>
+        <v>0</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V10" si="3">U3-T3</f>
-        <v>1</v>
+        <f t="shared" ref="V3:V10" si="2">U3-T3</f>
+        <v>0</v>
       </c>
       <c r="W3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -788,11 +785,11 @@
         <v>12</v>
       </c>
       <c r="Q4" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="R4" s="6">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
+        <f t="shared" ref="R4:R10" si="3">COUNTIF(B4:Q4, "W")/(COUNTIF(B4:Q4, "W")+COUNTIF(B4:Q4, "L"))</f>
+        <v>0.58333333333333337</v>
       </c>
       <c r="S4">
         <v>6</v>
@@ -802,12 +799,12 @@
         <v>0</v>
       </c>
       <c r="U4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V4">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V4">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4" t="s">
         <v>24</v>
@@ -863,11 +860,11 @@
         <v>12</v>
       </c>
       <c r="Q5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="R5" s="6">
-        <f t="shared" si="1"/>
-        <v>0.42857142857142855</v>
+        <f t="shared" si="3"/>
+        <v>0.55555555555555558</v>
       </c>
       <c r="S5">
         <v>6</v>
@@ -877,12 +874,12 @@
         <v>0</v>
       </c>
       <c r="U5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V5">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V5">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5" t="s">
         <v>9</v>
@@ -938,11 +935,11 @@
         <v>8</v>
       </c>
       <c r="Q6" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="R6" s="6">
-        <f t="shared" si="1"/>
-        <v>0.5714285714285714</v>
+        <f t="shared" si="3"/>
+        <v>0.5</v>
       </c>
       <c r="S6">
         <v>6</v>
@@ -952,12 +949,12 @@
         <v>0</v>
       </c>
       <c r="U6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V6">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V6">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6" t="s">
         <v>17</v>
@@ -1013,11 +1010,11 @@
         <v>12</v>
       </c>
       <c r="Q7" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="R7" s="6">
-        <f t="shared" si="1"/>
-        <v>0.625</v>
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S7">
         <v>6</v>
@@ -1027,12 +1024,12 @@
         <v>0</v>
       </c>
       <c r="U7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V7">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V7">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W7" t="s">
         <v>20</v>
@@ -1088,11 +1085,11 @@
         <v>12</v>
       </c>
       <c r="Q8" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="R8" s="6">
-        <f t="shared" si="1"/>
-        <v>0.875</v>
+        <f t="shared" si="3"/>
+        <v>0.88888888888888884</v>
       </c>
       <c r="S8">
         <v>6</v>
@@ -1102,12 +1099,12 @@
         <v>0</v>
       </c>
       <c r="U8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V8">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V8">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W8" t="s">
         <v>15</v>
@@ -1163,11 +1160,11 @@
         <v>12</v>
       </c>
       <c r="Q9" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="R9" s="6">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S9">
         <v>6</v>
@@ -1177,12 +1174,12 @@
         <v>0</v>
       </c>
       <c r="U9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V9">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V9">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9" t="s">
         <v>13</v>
@@ -1238,11 +1235,11 @@
         <v>10</v>
       </c>
       <c r="Q10" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="R10" s="6">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <f t="shared" si="3"/>
+        <v>0.54545454545454541</v>
       </c>
       <c r="S10">
         <v>6</v>
@@ -1252,12 +1249,12 @@
         <v>0</v>
       </c>
       <c r="U10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V10">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V10">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10" t="s">
         <v>22</v>
@@ -1327,13 +1324,13 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="Q11" s="5" t="e">
+      <c r="Q11" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.6</v>
       </c>
       <c r="R11" s="7">
-        <f>AVERAGEIF(B11:O11, "&gt;=0")</f>
-        <v>0.59615384615384615</v>
+        <f>AVERAGEIF(B11:Q11, "&gt;=0")</f>
+        <v>0.62333333333333329</v>
       </c>
       <c r="S11" s="2">
         <f>SUM(S3:S10)</f>
@@ -1345,16 +1342,16 @@
       </c>
       <c r="U11" s="2">
         <f>SUM(U3:U10)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="V11" s="2">
         <f>SUM(V3:V10)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1">
         <v>44803</v>
@@ -1488,11 +1485,11 @@
         <v>12</v>
       </c>
       <c r="Q15" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="R15" s="6">
-        <f t="shared" ref="R15:R20" si="7">COUNTIF(B15:O15, "W")/(COUNTIF(B15:O15, "W")+COUNTIF(B15:O15, "L"))</f>
-        <v>0.55555555555555558</v>
+        <f>COUNTIF(B15:Q15, "W")/(COUNTIF(B15:Q15, "W")+COUNTIF(B15:Q15, "L"))</f>
+        <v>0.6</v>
       </c>
       <c r="S15">
         <v>10</v>
@@ -1502,12 +1499,12 @@
         <v>0</v>
       </c>
       <c r="U15">
-        <f t="shared" ref="U15:U20" si="8">COUNTIF(B15:Q15, "A")</f>
-        <v>1</v>
+        <f t="shared" ref="U15:U20" si="7">COUNTIF(B15:Q15, "A")</f>
+        <v>0</v>
       </c>
       <c r="V15">
-        <f t="shared" ref="V15:V20" si="9">U15-T15</f>
-        <v>1</v>
+        <f t="shared" ref="V15:V20" si="8">U15-T15</f>
+        <v>0</v>
       </c>
       <c r="W15" t="s">
         <v>13</v>
@@ -1563,10 +1560,10 @@
         <v>10</v>
       </c>
       <c r="Q16" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="R16" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="R16:R22" si="9">COUNTIF(B16:Q16, "W")/(COUNTIF(B16:Q16, "W")+COUNTIF(B16:Q16, "L"))</f>
         <v>0.6</v>
       </c>
       <c r="S16">
@@ -1577,12 +1574,12 @@
         <v>0</v>
       </c>
       <c r="U16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V16">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="V16">
-        <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W16" t="s">
         <v>15</v>
@@ -1590,7 +1587,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -1638,11 +1635,11 @@
         <v>7</v>
       </c>
       <c r="Q17" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="R17" s="6">
-        <f t="shared" si="7"/>
-        <v>0.77777777777777779</v>
+        <f t="shared" si="9"/>
+        <v>0.7</v>
       </c>
       <c r="S17">
         <v>10</v>
@@ -1652,15 +1649,15 @@
         <v>0</v>
       </c>
       <c r="U17">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V17">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="V17">
-        <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -1713,11 +1710,11 @@
         <v>10</v>
       </c>
       <c r="Q18" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="R18" s="6">
-        <f t="shared" si="7"/>
-        <v>0.6</v>
+        <f t="shared" si="9"/>
+        <v>0.63636363636363635</v>
       </c>
       <c r="S18">
         <v>10</v>
@@ -1727,12 +1724,12 @@
         <v>0</v>
       </c>
       <c r="U18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V18">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="V18">
-        <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W18" t="s">
         <v>20</v>
@@ -1788,11 +1785,11 @@
         <v>12</v>
       </c>
       <c r="Q19" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="R19" s="6">
-        <f t="shared" si="7"/>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="9"/>
+        <v>0.45454545454545453</v>
       </c>
       <c r="S19">
         <v>10</v>
@@ -1802,12 +1799,12 @@
         <v>0</v>
       </c>
       <c r="U19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V19">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="V19">
-        <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W19" t="s">
         <v>22</v>
@@ -1815,7 +1812,7 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -1863,11 +1860,11 @@
         <v>8</v>
       </c>
       <c r="Q20" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="R20" s="6">
-        <f t="shared" si="7"/>
-        <v>0.5</v>
+        <f t="shared" si="9"/>
+        <v>0.42857142857142855</v>
       </c>
       <c r="S20">
         <v>6</v>
@@ -1877,20 +1874,20 @@
         <v>0</v>
       </c>
       <c r="U20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V20">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="V20">
-        <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
@@ -1938,11 +1935,11 @@
         <v>10</v>
       </c>
       <c r="Q21" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="R21" s="6">
-        <f>COUNTIF(B21:O21, "W")/(COUNTIF(B21:O21, "W")+COUNTIF(B21:O21, "L"))</f>
-        <v>0.8571428571428571</v>
+        <f t="shared" si="9"/>
+        <v>0.875</v>
       </c>
       <c r="S21">
         <v>6</v>
@@ -1953,19 +1950,19 @@
       </c>
       <c r="U21">
         <f>COUNTIF(B21:Q21, "A")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V21">
         <f>U21-T21</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -2013,11 +2010,11 @@
         <v>7</v>
       </c>
       <c r="Q22" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="R22" s="6">
-        <f>COUNTIF(B22:O22, "W")/(COUNTIF(B22:O22, "W")+COUNTIF(B22:O22, "L"))</f>
-        <v>0.5</v>
+        <f t="shared" si="9"/>
+        <v>0.41666666666666669</v>
       </c>
       <c r="S22">
         <v>10</v>
@@ -2028,14 +2025,14 @@
       </c>
       <c r="U22">
         <f>COUNTIF(B22:Q22, "A")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V22">
         <f>U22-T22</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
@@ -2102,13 +2099,13 @@
         <f t="shared" ref="P23" si="23">COUNTIF(P15:P22, "W")/(COUNTIF(P15:P22, "W")+COUNTIF(P15:P22, "L"))</f>
         <v>0.5</v>
       </c>
-      <c r="Q23" s="5" t="e">
+      <c r="Q23" s="5">
         <f t="shared" ref="Q23" si="24">COUNTIF(Q15:Q22, "W")/(COUNTIF(Q15:Q22, "W")+COUNTIF(Q15:Q22, "L"))</f>
-        <v>#DIV/0!</v>
+        <v>0.6</v>
       </c>
       <c r="R23" s="7">
-        <f>AVERAGEIF(B23:O23, "&gt;=0")</f>
-        <v>0.58571428571428563</v>
+        <f>AVERAGEIF(B23:Q23, "&gt;=0")</f>
+        <v>0.58124999999999993</v>
       </c>
       <c r="S23" s="2">
         <f>SUM(S15:S22)</f>
@@ -2120,11 +2117,11 @@
       </c>
       <c r="U23" s="2">
         <f>SUM(U15:U22)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="V23" s="2">
         <f>SUM(V15:V22)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>